<commit_message>
feat: update ragas calculation
</commit_message>
<xml_diff>
--- a/test/human/calc/calc_testcase.xlsx
+++ b/test/human/calc/calc_testcase.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Features\Documents\PMB-UNDIKSHA\va-pmb-undiksha\test\human\calc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08809422-3486-4943-86D4-94534B8D6C3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46F7F46B-2B15-4DFA-BB0F-9BF3F4B6C6E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1AD30FE2-C1F0-4340-B4CE-7F2C452643D4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{1AD30FE2-C1F0-4340-B4CE-7F2C452643D4}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="2" r:id="rId1"/>
@@ -151,15 +151,6 @@
     <t>P3</t>
   </si>
   <si>
-    <t>E1</t>
-  </si>
-  <si>
-    <t>E2</t>
-  </si>
-  <si>
-    <t>E3</t>
-  </si>
-  <si>
     <t>Apa jenis-jenis beasiswa bagi mahasiswa undiksha?</t>
   </si>
   <si>
@@ -1645,14 +1636,20 @@
   <si>
     <t>Presiden indonesia sekarang</t>
   </si>
+  <si>
+    <t>Eg1</t>
+  </si>
+  <si>
+    <t>Eg2</t>
+  </si>
+  <si>
+    <t>Eg3</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.000"/>
-  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1842,9 +1839,6 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1901,6 +1895,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2109,7 +2106,7 @@
                   <c:v>0.98449999999999993</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.85895356173206849</c:v>
+                  <c:v>0.85901560927639264</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2706,6 +2703,38 @@
         <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-ID" sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Test case</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2803,6 +2832,38 @@
           </c:spPr>
         </c:majorGridlines>
         <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-ID" sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Range Score</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4067,7 +4128,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Metric Answer Relevancy</a:t>
+              <a:t>Metric Response Relevancy</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -4146,154 +4207,154 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="50"/>
                 <c:pt idx="0">
-                  <c:v>0.76161836422559015</c:v>
+                  <c:v>0.76170501431540105</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.80981242725785707</c:v>
+                  <c:v>0.80982548427416268</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.83514468342650094</c:v>
+                  <c:v>0.83688674310992839</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.86458597213040633</c:v>
+                  <c:v>0.86440026625069288</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.88465388518011823</c:v>
+                  <c:v>0.88471054302820085</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.75251901721403536</c:v>
+                  <c:v>0.75253946345172784</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.8866737706229525</c:v>
+                  <c:v>0.88680199748219468</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.80686434727441536</c:v>
+                  <c:v>0.80687199784055386</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.93993134247215782</c:v>
+                  <c:v>0.93998011626732092</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.93523266766798585</c:v>
+                  <c:v>0.93525161069690499</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.89212733483162632</c:v>
+                  <c:v>0.89212951300674115</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.84203095228593605</c:v>
+                  <c:v>0.84189822952653703</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.73663916821675501</c:v>
+                  <c:v>0.73657402592247434</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.88781938404459682</c:v>
+                  <c:v>0.88771553966581873</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.80737215410506724</c:v>
+                  <c:v>0.80731691451692333</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.92110747728249842</c:v>
+                  <c:v>0.92109329220621516</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.84240318019841531</c:v>
+                  <c:v>0.84238246917305259</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.90861149892977655</c:v>
+                  <c:v>0.90858932692763583</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.98393779246242963</c:v>
+                  <c:v>0.98392905363163141</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.90589808620165668</c:v>
+                  <c:v>0.90590848904502597</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.90722929012872067</c:v>
+                  <c:v>0.9057018862402858</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.88079742797158322</c:v>
+                  <c:v>0.88081710646046896</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.90398218744704073</c:v>
+                  <c:v>0.90398912279127719</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.91278270936526518</c:v>
+                  <c:v>0.91277938856830299</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.89740984316424888</c:v>
+                  <c:v>0.89740545995089072</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.85765631180053636</c:v>
+                  <c:v>0.85764525606298514</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.80835165541589804</c:v>
+                  <c:v>0.80837504653803505</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.85762618539985291</c:v>
+                  <c:v>0.85763782968575064</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.79808500519814196</c:v>
+                  <c:v>0.79821532354210234</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.76498113648651545</c:v>
+                  <c:v>0.76496760527611352</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.93230215379142456</c:v>
+                  <c:v>0.93229094456408834</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.83739388934779713</c:v>
+                  <c:v>0.83737568331669265</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.86749421843900942</c:v>
+                  <c:v>0.86750100737364522</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.92264341210748446</c:v>
+                  <c:v>0.92350748740114508</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.94588845514064757</c:v>
+                  <c:v>0.94589752223457113</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.91361593344481296</c:v>
+                  <c:v>0.91360048047282294</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.93708351189708783</c:v>
+                  <c:v>0.93707892837099604</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.91251529745747506</c:v>
+                  <c:v>0.91213227117131213</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.91984578532538774</c:v>
+                  <c:v>0.92073411265131877</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.90421514187619323</c:v>
+                  <c:v>0.90426964391318876</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.84215580800103174</c:v>
+                  <c:v>0.84218185253416122</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.72403530366222046</c:v>
+                  <c:v>0.72353714308184769</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.75774846619959868</c:v>
+                  <c:v>0.75768426389999333</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.86146536113098537</c:v>
+                  <c:v>0.86146988108181777</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.77363764764003851</c:v>
+                  <c:v>0.77264097600753201</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.95667021727558399</c:v>
+                  <c:v>0.95658971765814937</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.88285224592408651</c:v>
+                  <c:v>0.88289961446655563</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.78729805785175022</c:v>
+                  <c:v>0.79038940653951562</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.99561631730143807</c:v>
+                  <c:v>0.99562344630014488</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.47931560438079135</c:v>
+                  <c:v>0.47933196532479122</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7850,33 +7911,33 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
+      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="67.42578125" customWidth="1"/>
+    <col min="2" max="5" width="37.5703125" customWidth="1"/>
     <col min="6" max="9" width="45.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="22" t="s">
+      <c r="A1" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22" t="s">
+      <c r="C1" s="21"/>
+      <c r="D1" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="22"/>
+      <c r="E1" s="21"/>
     </row>
     <row r="2" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="24"/>
+      <c r="A2" s="23"/>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
@@ -7884,7 +7945,7 @@
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>2</v>
@@ -7895,16 +7956,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="14" customFormat="1" ht="375" x14ac:dyDescent="0.25">
@@ -7912,16 +7973,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="14" customFormat="1" ht="90" x14ac:dyDescent="0.25">
@@ -7929,16 +7990,16 @@
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="14" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -7946,16 +8007,16 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="14" customFormat="1" ht="180" x14ac:dyDescent="0.25">
@@ -7963,16 +8024,16 @@
         <v>5</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="14" customFormat="1" ht="135" x14ac:dyDescent="0.25">
@@ -7980,16 +8041,16 @@
         <v>6</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="14" customFormat="1" ht="315" x14ac:dyDescent="0.25">
@@ -7997,16 +8058,16 @@
         <v>7</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="14" customFormat="1" ht="120" x14ac:dyDescent="0.25">
@@ -8014,16 +8075,16 @@
         <v>8</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="14" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -8031,16 +8092,16 @@
         <v>9</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:5" s="14" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
@@ -8048,16 +8109,16 @@
         <v>10</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="13" spans="1:5" s="14" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -8065,16 +8126,16 @@
         <v>11</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:5" s="14" customFormat="1" ht="90" x14ac:dyDescent="0.25">
@@ -8082,16 +8143,16 @@
         <v>12</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:5" s="14" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -8099,16 +8160,16 @@
         <v>13</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="16" spans="1:5" s="14" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -8116,16 +8177,16 @@
         <v>14</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:5" s="14" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -8133,16 +8194,16 @@
         <v>15</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="18" spans="1:5" s="14" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -8150,16 +8211,16 @@
         <v>16</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="19" spans="1:5" s="14" customFormat="1" ht="90" x14ac:dyDescent="0.25">
@@ -8167,16 +8228,16 @@
         <v>17</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="20" spans="1:5" s="14" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -8184,16 +8245,16 @@
         <v>18</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="21" spans="1:5" s="14" customFormat="1" ht="90" x14ac:dyDescent="0.25">
@@ -8201,16 +8262,16 @@
         <v>19</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="22" spans="1:5" s="14" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -8218,16 +8279,16 @@
         <v>20</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="23" spans="1:5" s="14" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -8235,16 +8296,16 @@
         <v>21</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="24" spans="1:5" s="14" customFormat="1" ht="90" x14ac:dyDescent="0.25">
@@ -8252,16 +8313,16 @@
         <v>22</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="25" spans="1:5" s="14" customFormat="1" ht="90" x14ac:dyDescent="0.25">
@@ -8269,16 +8330,16 @@
         <v>23</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="26" spans="1:5" s="14" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -8286,16 +8347,16 @@
         <v>24</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="27" spans="1:5" s="14" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
@@ -8303,16 +8364,16 @@
         <v>25</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="28" spans="1:5" s="14" customFormat="1" ht="240" x14ac:dyDescent="0.25">
@@ -8320,16 +8381,16 @@
         <v>26</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="29" spans="1:5" s="14" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -8337,16 +8398,16 @@
         <v>27</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="30" spans="1:5" s="14" customFormat="1" ht="195" x14ac:dyDescent="0.25">
@@ -8354,16 +8415,16 @@
         <v>28</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="31" spans="1:5" s="14" customFormat="1" ht="120" x14ac:dyDescent="0.25">
@@ -8371,16 +8432,16 @@
         <v>29</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="32" spans="1:5" s="14" customFormat="1" ht="135" x14ac:dyDescent="0.25">
@@ -8388,16 +8449,16 @@
         <v>30</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="33" spans="1:5" s="14" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -8405,16 +8466,16 @@
         <v>31</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="34" spans="1:5" s="14" customFormat="1" ht="285" x14ac:dyDescent="0.25">
@@ -8422,16 +8483,16 @@
         <v>32</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="35" spans="1:5" s="14" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -8439,16 +8500,16 @@
         <v>33</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="36" spans="1:5" s="14" customFormat="1" ht="225" x14ac:dyDescent="0.25">
@@ -8456,16 +8517,16 @@
         <v>34</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="37" spans="1:5" s="14" customFormat="1" ht="195" x14ac:dyDescent="0.25">
@@ -8473,16 +8534,16 @@
         <v>35</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="38" spans="1:5" s="14" customFormat="1" ht="165" x14ac:dyDescent="0.25">
@@ -8490,16 +8551,16 @@
         <v>36</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="39" spans="1:5" s="14" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -8507,16 +8568,16 @@
         <v>37</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="40" spans="1:5" s="14" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
@@ -8524,16 +8585,16 @@
         <v>38</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="41" spans="1:5" s="14" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
@@ -8541,16 +8602,16 @@
         <v>39</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="42" spans="1:5" s="14" customFormat="1" ht="255" x14ac:dyDescent="0.25">
@@ -8558,16 +8619,16 @@
         <v>40</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="43" spans="1:5" s="14" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -8575,16 +8636,16 @@
         <v>41</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="44" spans="1:5" s="14" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -8592,16 +8653,16 @@
         <v>42</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="45" spans="1:5" s="14" customFormat="1" ht="195" x14ac:dyDescent="0.25">
@@ -8609,16 +8670,16 @@
         <v>43</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="46" spans="1:5" s="14" customFormat="1" ht="105" x14ac:dyDescent="0.25">
@@ -8626,16 +8687,16 @@
         <v>44</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="47" spans="1:5" s="14" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -8643,16 +8704,16 @@
         <v>45</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="48" spans="1:5" s="14" customFormat="1" ht="210" x14ac:dyDescent="0.25">
@@ -8660,16 +8721,16 @@
         <v>46</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="49" spans="1:5" s="14" customFormat="1" ht="285" x14ac:dyDescent="0.25">
@@ -8677,16 +8738,16 @@
         <v>47</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="50" spans="1:5" s="14" customFormat="1" ht="285" x14ac:dyDescent="0.25">
@@ -8694,16 +8755,16 @@
         <v>48</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="51" spans="1:5" s="14" customFormat="1" ht="210" x14ac:dyDescent="0.25">
@@ -8711,16 +8772,16 @@
         <v>49</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="52" spans="1:5" s="14" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -8728,16 +8789,16 @@
         <v>50</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -8759,7 +8820,7 @@
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
+      <selection pane="bottomLeft" activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8785,16 +8846,16 @@
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>17</v>
@@ -10911,27 +10972,27 @@
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="26"/>
-      <c r="B52" s="27"/>
-      <c r="C52" s="27"/>
-      <c r="D52" s="27"/>
-      <c r="E52" s="27"/>
-      <c r="F52" s="27"/>
-      <c r="G52" s="27"/>
-      <c r="H52" s="27"/>
-      <c r="I52" s="28"/>
+      <c r="A52" s="25"/>
+      <c r="B52" s="26"/>
+      <c r="C52" s="26"/>
+      <c r="D52" s="26"/>
+      <c r="E52" s="26"/>
+      <c r="F52" s="26"/>
+      <c r="G52" s="26"/>
+      <c r="H52" s="26"/>
+      <c r="I52" s="27"/>
     </row>
     <row r="53" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A53" s="25" t="s">
-        <v>230</v>
-      </c>
-      <c r="B53" s="25"/>
-      <c r="C53" s="25"/>
-      <c r="D53" s="25"/>
-      <c r="E53" s="25"/>
-      <c r="F53" s="25"/>
-      <c r="G53" s="25"/>
-      <c r="H53" s="25"/>
+      <c r="A53" s="24" t="s">
+        <v>227</v>
+      </c>
+      <c r="B53" s="24"/>
+      <c r="C53" s="24"/>
+      <c r="D53" s="24"/>
+      <c r="E53" s="24"/>
+      <c r="F53" s="24"/>
+      <c r="G53" s="24"/>
+      <c r="H53" s="24"/>
       <c r="I53" s="11">
         <f>IFERROR(AVERAGE(I2:I51),0)</f>
         <v>1</v>
@@ -10952,8 +11013,8 @@
   <dimension ref="A1:H53"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I11" sqref="I11"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10977,7 +11038,7 @@
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -12850,25 +12911,25 @@
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="26"/>
-      <c r="B52" s="27"/>
-      <c r="C52" s="27"/>
-      <c r="D52" s="27"/>
-      <c r="E52" s="27"/>
-      <c r="F52" s="27"/>
-      <c r="G52" s="27"/>
-      <c r="H52" s="28"/>
+      <c r="A52" s="25"/>
+      <c r="B52" s="26"/>
+      <c r="C52" s="26"/>
+      <c r="D52" s="26"/>
+      <c r="E52" s="26"/>
+      <c r="F52" s="26"/>
+      <c r="G52" s="26"/>
+      <c r="H52" s="27"/>
     </row>
     <row r="53" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A53" s="29" t="s">
-        <v>230</v>
-      </c>
-      <c r="B53" s="30"/>
-      <c r="C53" s="30"/>
-      <c r="D53" s="30"/>
-      <c r="E53" s="30"/>
-      <c r="F53" s="30"/>
-      <c r="G53" s="31"/>
+      <c r="A53" s="28" t="s">
+        <v>227</v>
+      </c>
+      <c r="B53" s="29"/>
+      <c r="C53" s="29"/>
+      <c r="D53" s="29"/>
+      <c r="E53" s="29"/>
+      <c r="F53" s="29"/>
+      <c r="G53" s="30"/>
       <c r="H53" s="11">
         <f>IFERROR(AVERAGE(H2:H51),0)</f>
         <v>1</v>
@@ -12886,25 +12947,24 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29B313D2-6D9A-4745-AFAD-8265468567C4}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:H53"/>
+  <dimension ref="A1:H56"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J19" sqref="J19"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J61" sqref="J61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.5703125" style="2" customWidth="1"/>
     <col min="2" max="5" width="22.85546875" customWidth="1"/>
-    <col min="6" max="6" width="97.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="56.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.5703125" style="2" customWidth="1"/>
+    <col min="6" max="7" width="38.140625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" style="2" customWidth="1"/>
     <col min="11" max="12" width="23.5703125" customWidth="1"/>
     <col min="13" max="13" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="56.25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -12915,18 +12975,18 @@
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="38" t="s">
         <v>22</v>
       </c>
     </row>
@@ -14788,29 +14848,35 @@
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="26"/>
-      <c r="B52" s="27"/>
-      <c r="C52" s="27"/>
-      <c r="D52" s="27"/>
-      <c r="E52" s="27"/>
-      <c r="F52" s="27"/>
-      <c r="G52" s="27"/>
-      <c r="H52" s="28"/>
+      <c r="A52" s="25"/>
+      <c r="B52" s="26"/>
+      <c r="C52" s="26"/>
+      <c r="D52" s="26"/>
+      <c r="E52" s="26"/>
+      <c r="F52" s="26"/>
+      <c r="G52" s="26"/>
+      <c r="H52" s="27"/>
     </row>
     <row r="53" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A53" s="25" t="s">
-        <v>230</v>
-      </c>
-      <c r="B53" s="25"/>
-      <c r="C53" s="25"/>
-      <c r="D53" s="25"/>
-      <c r="E53" s="25"/>
-      <c r="F53" s="25"/>
-      <c r="G53" s="25"/>
+      <c r="A53" s="24" t="s">
+        <v>227</v>
+      </c>
+      <c r="B53" s="24"/>
+      <c r="C53" s="24"/>
+      <c r="D53" s="24"/>
+      <c r="E53" s="24"/>
+      <c r="F53" s="24"/>
+      <c r="G53" s="24"/>
       <c r="H53" s="11">
         <f>IFERROR(AVERAGE(H2:H51),0)</f>
         <v>0.98449999999999993</v>
       </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H55" s="17"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H56" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -14824,11 +14890,11 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8D66942-FB14-40F2-914A-71EA8DF8C59E}">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:L53"/>
+  <dimension ref="A1:L57"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M11" sqref="M11"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14853,7 +14919,7 @@
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -14868,13 +14934,13 @@
         <v>28</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>29</v>
+        <v>361</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>30</v>
+        <v>362</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>31</v>
+        <v>363</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>23</v>
@@ -14928,26 +14994,26 @@
 Beasiswa ini ditujukan untuk mahasiswa berprestasi maupun mahasiswa kurang mampu, dan pengelolaan, pendaftaran, serta seleksi beasiswa diselenggarakan secara online maupun offline.</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="I2" s="4">
-        <v>0.71831101491732086</v>
+        <v>0.71851097526223429</v>
       </c>
       <c r="J2" s="4">
-        <v>0.57395121376414759</v>
+        <v>0.57400950636733272</v>
       </c>
       <c r="K2" s="4">
-        <v>0.99259286399530189</v>
+        <v>0.99259456131663648</v>
       </c>
       <c r="L2" s="7">
         <f>IFERROR(AVERAGE(I2:K2),0)</f>
-        <v>0.76161836422559015</v>
+        <v>0.76170501431540105</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -14979,26 +15045,26 @@
 Untuk informasi lebih lanjut, Anda dapat mengunjungi website resmi program Adik Papua di [https://adik.kemdikbud.go.id](https://adik.kemdikbud.go.id).</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="I3" s="4">
-        <v>0.6340385890092699</v>
+        <v>0.63398969710269693</v>
       </c>
       <c r="J3" s="4">
-        <v>0.98221489014848062</v>
+        <v>0.98225009655464013</v>
       </c>
       <c r="K3" s="4">
-        <v>0.81318380261582068</v>
+        <v>0.81323665916515109</v>
       </c>
       <c r="L3" s="7">
         <f t="shared" ref="L3:L51" si="0">IFERROR(AVERAGE(I3:K3),0)</f>
-        <v>0.80981242725785707</v>
+        <v>0.80982548427416268</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -15020,26 +15086,26 @@
 Anda dapat melihat informasi daya tampung mahasiswa baru Universitas Pendidikan Ganesha tahun akademik 2024/2025 dengan mengunjungi tautan berikut: [Daya Tampung Mahasiswa Baru Tahun Akademik 2024/2025](https://undiksha.ac.id/pmb/tahun2024/daya-tampung/).</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="I4" s="4">
-        <v>0.85239646118902157</v>
+        <v>0.85263439567443</v>
       </c>
       <c r="J4" s="4">
-        <v>0.67711247506006267</v>
+        <v>0.67934954361236399</v>
       </c>
       <c r="K4" s="4">
-        <v>0.97592511403041871</v>
+        <v>0.97867629004299117</v>
       </c>
       <c r="L4" s="7">
         <f t="shared" si="0"/>
-        <v>0.83514468342650094</v>
+        <v>0.83688674310992839</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -15061,26 +15127,26 @@
 Daya tampung mahasiswa untuk Program Studi Ilmu Komputer (S1) di Universitas Pendidikan Ganesha adalah 110 mahasiswa.</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="I5" s="4">
-        <v>0.83909561864858062</v>
+        <v>0.83679804265726865</v>
       </c>
       <c r="J5" s="4">
-        <v>0.78455398775758178</v>
+        <v>0.78558497392701299</v>
       </c>
       <c r="K5" s="4">
-        <v>0.9701083099850567</v>
+        <v>0.97081778216779702</v>
       </c>
       <c r="L5" s="7">
         <f t="shared" si="0"/>
-        <v>0.86458597213040633</v>
+        <v>0.86440026625069288</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -15112,26 +15178,26 @@
 Jika ada pertanyaan lebih lanjut, silakan tanyakan!</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="I6" s="4">
-        <v>0.80730674802742919</v>
+        <v>0.80743659739000839</v>
       </c>
       <c r="J6" s="4">
-        <v>1</v>
+        <v>0.99999872724177241</v>
       </c>
       <c r="K6" s="4">
-        <v>0.84665490751292549</v>
+        <v>0.84669630445282174</v>
       </c>
       <c r="L6" s="7">
         <f t="shared" si="0"/>
-        <v>0.88465388518011823</v>
+        <v>0.88471054302820085</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -15153,26 +15219,26 @@
 Estimasi biaya kuliah adalah perkiraan biaya yang harus ditanggung oleh calon mahasiswa per semester untuk mengikuti perkuliahan di Universitas Pendidikan Ganesha (Undiksha). Biaya ini mencakup berbagai komponen, seperti biaya pendidikan, biaya administrasi, dan biaya lainnya yang terkait dengan proses belajar mengajar. Estimasi ini penting untuk membantu calon mahasiswa merencanakan keuangan mereka selama menempuh pendidikan di Undiksha.</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="I7" s="4">
-        <v>0.95751801957410598</v>
+        <v>0.95746545948414052</v>
       </c>
       <c r="J7" s="4">
-        <v>0.63899458159745859</v>
+        <v>0.63899285125630156</v>
       </c>
       <c r="K7" s="4">
-        <v>0.66104445047054139</v>
+        <v>0.66116007961474155</v>
       </c>
       <c r="L7" s="7">
         <f t="shared" si="0"/>
-        <v>0.75251901721403536</v>
+        <v>0.75253946345172784</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -15234,26 +15300,26 @@
 Fasilitas-fasilitas ini dirancang untuk mendukung kegiatan akademik dan non-akademik di Undiksha.</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="I8" s="4">
-        <v>0.80235835678389067</v>
+        <v>0.80288984253684315</v>
       </c>
       <c r="J8" s="4">
-        <v>0.98662642028050451</v>
+        <v>0.98650429819918339</v>
       </c>
       <c r="K8" s="4">
-        <v>0.87103653480446208</v>
+        <v>0.87101185171055751</v>
       </c>
       <c r="L8" s="7">
         <f t="shared" si="0"/>
-        <v>0.8866737706229525</v>
+        <v>0.88680199748219468</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -15275,26 +15341,26 @@
 Anda dapat mendapatkan informasi mengenai fasilitas layanan konseling di Universitas Pendidikan Ganesha dengan menghubungi unit konseling yang tersedia. Layanan ini ditangani oleh konselor yang berpengalaman dan dapat membantu mahasiswa dalam memecahkan masalah akademik dan non akademik. Untuk informasi lebih lanjut, Anda dapat menghubungi nomor berikut: (+6281246318813).</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="I9" s="4">
-        <v>0.70492986829673887</v>
+        <v>0.70499335675751873</v>
       </c>
       <c r="J9" s="4">
-        <v>0.74092930961996006</v>
+        <v>0.74097428963356093</v>
       </c>
       <c r="K9" s="4">
-        <v>0.97473386390654693</v>
+        <v>0.9746483471305819</v>
       </c>
       <c r="L9" s="7">
         <f t="shared" si="0"/>
-        <v>0.80686434727441536</v>
+        <v>0.80687199784055386</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -15316,26 +15382,26 @@
 Dekan Fakultas Bahasa dan Seni (FBS) Universitas Pendidikan Ganesha adalah Drs. I Gede Nurjaya, M.Pd.</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="I10" s="4">
-        <v>0.99999865335974392</v>
+        <v>0.99999884088833302</v>
       </c>
       <c r="J10" s="4">
-        <v>0.97205187705583351</v>
+        <v>0.97207992813888155</v>
       </c>
       <c r="K10" s="4">
-        <v>0.8477434970008958</v>
+        <v>0.84786157977474808</v>
       </c>
       <c r="L10" s="7">
         <f t="shared" si="0"/>
-        <v>0.93993134247215782</v>
+        <v>0.93998011626732092</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -15423,26 +15489,26 @@
 Jika Anda memerlukan informasi lebih lanjut, silakan menghubungi kontak yang tertera.</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="I11" s="4">
-        <v>0.91677694745222271</v>
+        <v>0.91685376598194201</v>
       </c>
       <c r="J11" s="4">
-        <v>0.91147775022880162</v>
+        <v>0.91146521955325421</v>
       </c>
       <c r="K11" s="4">
-        <v>0.97744330532293322</v>
+        <v>0.97743584655551841</v>
       </c>
       <c r="L11" s="7">
         <f t="shared" si="0"/>
-        <v>0.93523266766798585</v>
+        <v>0.93525161069690499</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -15464,26 +15530,26 @@
 Nama Wakil Dekan I Fakultas Ekonomi (FE) Universitas Pendidikan Ganesha adalah Dr. Dra. Ni Made Suci, M.Si.</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="I12" s="4">
-        <v>0.99999894714986659</v>
+        <v>0.99999916495249463</v>
       </c>
       <c r="J12" s="4">
-        <v>0.814604623592868</v>
+        <v>0.81456933031344625</v>
       </c>
       <c r="K12" s="4">
-        <v>0.86177843375214425</v>
+        <v>0.86182004375428245</v>
       </c>
       <c r="L12" s="7">
         <f t="shared" si="0"/>
-        <v>0.89212733483162632</v>
+        <v>0.89212951300674115</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -15507,26 +15573,26 @@
 "Menjadi Fakultas Unggul Berjiwa Wirausaha Berlandaskan Falsafah Tri Hita Karana di Asia Tahun 2045."</v>
       </c>
       <c r="F13" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="G13" s="5" t="s">
         <v>273</v>
       </c>
-      <c r="G13" s="5" t="s">
-        <v>276</v>
-      </c>
       <c r="H13" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I13" s="4">
-        <v>0.70915444558903495</v>
+        <v>0.70889882841642027</v>
       </c>
       <c r="J13" s="4">
-        <v>0.81693980976707925</v>
+        <v>0.81679710638981995</v>
       </c>
       <c r="K13" s="4">
-        <v>0.99999860150169417</v>
+        <v>0.999998753773371</v>
       </c>
       <c r="L13" s="7">
         <f t="shared" si="0"/>
-        <v>0.84203095228593605</v>
+        <v>0.84189822952653703</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -15548,26 +15614,26 @@
 Anda dapat mengunjungi website Fakultas Hukum dan Ilmu Sosial Universitas Pendidikan Ganesha (Undiksha) melalui tautan berikut: [fhis.undiksha.ac.id](http://fhis.undiksha.ac.id). Di sana, Anda dapat menemukan informasi terkait program studi, kegiatan, dan berita terbaru dari fakultas tersebut.</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="I14" s="4">
-        <v>0.73465914274376787</v>
+        <v>0.73455558948689359</v>
       </c>
       <c r="J14" s="4">
-        <v>0.79013610728675732</v>
+        <v>0.79012014400078334</v>
       </c>
       <c r="K14" s="4">
-        <v>0.68512225461973975</v>
+        <v>0.68504634427974564</v>
       </c>
       <c r="L14" s="7">
         <f t="shared" si="0"/>
-        <v>0.73663916821675501</v>
+        <v>0.73657402592247434</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -15589,26 +15655,26 @@
 Ya, Fakultas Hukum dan Ilmu Sosial (FHIS) Universitas Pendidikan Ganesha memiliki video profil. Anda dapat menontonnya melalui tautan berikut: [Video Profil FHIS Undiksha](https://youtu.be/xrruGWs5HNk). Video ini memberikan informasi mengenai fakultas, program studi, dan berbagai kegiatan yang ada di FHIS.</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="I15" s="4">
-        <v>0.91968023667619558</v>
+        <v>0.91940527532188354</v>
       </c>
       <c r="J15" s="4">
-        <v>0.74377791545759486</v>
+        <v>0.74374201013075392</v>
       </c>
       <c r="K15" s="4">
-        <v>1</v>
+        <v>0.99999933354481896</v>
       </c>
       <c r="L15" s="7">
         <f t="shared" si="0"/>
-        <v>0.88781938404459682</v>
+        <v>0.88771553966581873</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -15630,26 +15696,26 @@
 Nama dekan Fakultas Ilmu Pendidikan (FIP) Universitas Pendidikan Ganesha adalah Prof. Dr. I Wayan Widiana, S.Pd., M.Pd.</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="I16" s="4">
-        <v>0.80206499390473862</v>
+        <v>0.80210401758350769</v>
       </c>
       <c r="J16" s="4">
-        <v>0.86781613394152313</v>
+        <v>0.86789705690993957</v>
       </c>
       <c r="K16" s="4">
-        <v>0.75223533446893998</v>
+        <v>0.75194966905732308</v>
       </c>
       <c r="L16" s="7">
         <f t="shared" si="0"/>
-        <v>0.80737215410506724</v>
+        <v>0.80731691451692333</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -15671,26 +15737,26 @@
 Fakultas Ilmu Pendidikan (FIP) Universitas Pendidikan Ganesha mulai berdiri pada tahun 1968. Jurusan awal yang ada di FIP adalah Jurusan Bimbingan dan Penyuluhan serta Pendidikan Luar Sekolah.</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="I17" s="4">
-        <v>0.81466543237126066</v>
+        <v>0.81459532841910676</v>
       </c>
       <c r="J17" s="4">
-        <v>0.96353700566584699</v>
+        <v>0.96359529368819141</v>
       </c>
       <c r="K17" s="4">
-        <v>0.98511999381038717</v>
+        <v>0.98508925451134755</v>
       </c>
       <c r="L17" s="7">
         <f t="shared" si="0"/>
-        <v>0.92110747728249842</v>
+        <v>0.92109329220621516</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -15712,26 +15778,26 @@
 Fakultas Kedokteran Universitas Pendidikan Ganesha (Undiksha) didirikan berdasarkan Keputusan Menteri Riset Teknologi dan Pendidikan Tinggi Republik Indonesia, Nomor: 574/KPT/I/2018 tertanggal 16 Juli 2018.</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="I18" s="4">
-        <v>0.68778009311369537</v>
+        <v>0.68778765013690857</v>
       </c>
       <c r="J18" s="4">
-        <v>0.99999906671709426</v>
+        <v>1</v>
       </c>
       <c r="K18" s="4">
-        <v>0.83943038076445631</v>
+        <v>0.83935975738224944</v>
       </c>
       <c r="L18" s="7">
         <f t="shared" si="0"/>
-        <v>0.84240318019841531</v>
+        <v>0.84238246917305259</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -15753,26 +15819,26 @@
 Visi Fakultas Kedokteran (FK) Universitas Pendidikan Ganesha adalah menjadi program studi kedokteran unggul dalam bidang kedokteran pariwisata berlandaskan Falsafah Tri Hita Karana di Asia Tahun 2045.</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="I19" s="4">
-        <v>0.95128867872625278</v>
+        <v>0.95119631223481382</v>
       </c>
       <c r="J19" s="4">
-        <v>0.95969793392085967</v>
+        <v>0.95969803208392712</v>
       </c>
       <c r="K19" s="4">
-        <v>0.81484788414221709</v>
+        <v>0.81487363646416644</v>
       </c>
       <c r="L19" s="7">
         <f t="shared" si="0"/>
-        <v>0.90861149892977655</v>
+        <v>0.90858932692763583</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -15794,26 +15860,26 @@
 Visi Fakultas Matematika dan Ilmu Pengetahuan Alam (MIPA) Universitas Pendidikan Ganesha adalah: "Menjadi Fakultas Unggul Dalam Matematika Dan Ilmu Pengetahuan Alam Berlandaskan Falsafah Tri Hita Karana Di Asia Tahun 2045."</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="I20" s="4">
-        <v>0.99999878555452226</v>
+        <v>0.99999879815464598</v>
       </c>
       <c r="J20" s="4">
-        <v>0.96895050497178148</v>
+        <v>0.96894380154297011</v>
       </c>
       <c r="K20" s="4">
-        <v>0.98286408686098536</v>
+        <v>0.98284456119727803</v>
       </c>
       <c r="L20" s="7">
         <f t="shared" si="0"/>
-        <v>0.98393779246242963</v>
+        <v>0.98392905363163141</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -15835,26 +15901,26 @@
 Dekan Fakultas Matematika dan Ilmu Pengetahuan Alam (FMIPA) Universitas Pendidikan Ganesha adalah Dr. I Wayan Sukra Warpala, S.Pd., M.Sc.</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="I21" s="4">
-        <v>0.95217180126746492</v>
+        <v>0.95235811537844794</v>
       </c>
       <c r="J21" s="4">
-        <v>0.81914610242761399</v>
+        <v>0.81900866839372355</v>
       </c>
       <c r="K21" s="4">
-        <v>0.94637635490989092</v>
+        <v>0.94635868336290629</v>
       </c>
       <c r="L21" s="7">
         <f t="shared" si="0"/>
-        <v>0.90589808620165668</v>
+        <v>0.90590848904502597</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -15876,26 +15942,26 @@
 Program Studi Pendidikan Olahraga dan Kesehatan pertama kali berdiri pada tahun 1988 di bawah Jurusan Pendidikan Matematika dan Ilmu Pengetahuan Alam (MIPA).</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="I22" s="4">
-        <v>0.95955518803330386</v>
+        <v>0.95899259792947289</v>
       </c>
       <c r="J22" s="4">
-        <v>0.88978460640114898</v>
+        <v>0.88896052744723941</v>
       </c>
       <c r="K22" s="4">
-        <v>0.87234807595170916</v>
+        <v>0.869152533344145</v>
       </c>
       <c r="L22" s="7">
         <f t="shared" si="0"/>
-        <v>0.90722929012872067</v>
+        <v>0.9057018862402858</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -15917,26 +15983,26 @@
 Visi Fakultas Olahraga dan Kesehatan (FOK) Universitas Pendidikan Ganesha adalah menjadi Fakultas unggul dalam menghasilkan Sumber Daya Manusia (SDM) di bidang keolahragaan dan kesehatan berlandaskan falsafah Tri Hita Karana di Indonesia tahun 2045.</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="I23" s="4">
-        <v>0.97034120086047149</v>
+        <v>0.97037868093137847</v>
       </c>
       <c r="J23" s="4">
-        <v>0.83858906036836567</v>
+        <v>0.83853449535206503</v>
       </c>
       <c r="K23" s="4">
-        <v>0.83346202268591263</v>
+        <v>0.83353814309796359</v>
       </c>
       <c r="L23" s="7">
         <f t="shared" si="0"/>
-        <v>0.88079742797158322</v>
+        <v>0.88081710646046896</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -15958,26 +16024,26 @@
 Fakultas Teknik dan Kejuruan (FTK) Universitas Pendidikan Ganesha mulai berdiri pada tahun 1990. Program studi awal yang ditawarkan adalah Pendidikan Kesejahteraan Keluarga di bawah Jurusan Ilmu Pendidikan.</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="I24" s="4">
-        <v>0.98542628311114666</v>
+        <v>0.98541505648305294</v>
       </c>
       <c r="J24" s="4">
-        <v>0.78842603148624557</v>
+        <v>0.7883865281671999</v>
       </c>
       <c r="K24" s="4">
-        <v>0.93809424774372996</v>
+        <v>0.93816578372357884</v>
       </c>
       <c r="L24" s="7">
         <f t="shared" si="0"/>
-        <v>0.90398218744704073</v>
+        <v>0.90398912279127719</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -15999,26 +16065,26 @@
 Dekan Fakultas Teknik dan Kejuruan (FTK) Universitas Pendidikan Ganesha adalah Dr. Kadek Rihendra Dantes, S.T., M.T.</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="I25" s="4">
-        <v>0.95908974761021237</v>
+        <v>0.95909082456105632</v>
       </c>
       <c r="J25" s="4">
-        <v>0.84223752912389305</v>
+        <v>0.84223654566915118</v>
       </c>
       <c r="K25" s="4">
-        <v>0.93702085136168989</v>
+        <v>0.93701079547470167</v>
       </c>
       <c r="L25" s="7">
         <f t="shared" si="0"/>
-        <v>0.91278270936526518</v>
+        <v>0.91277938856830299</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -16052,26 +16118,26 @@
 Pengembangan kurikulum di Undiksha bertujuan untuk menghasilkan lulusan yang kompeten dan siap menghadapi tantangan di dunia kerja serta berkontribusi pada masyarakat.</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="I26" s="4">
-        <v>0.88405122987654938</v>
+        <v>0.88403011190425518</v>
       </c>
       <c r="J26" s="4">
-        <v>0.88663300839723813</v>
+        <v>0.88652011910706408</v>
       </c>
       <c r="K26" s="4">
-        <v>0.92154529121895912</v>
+        <v>0.92166614884135301</v>
       </c>
       <c r="L26" s="7">
         <f t="shared" si="0"/>
-        <v>0.89740984316424888</v>
+        <v>0.89740545995089072</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -16106,26 +16172,26 @@
 Keempat jenis kecerdasan ini bertujuan untuk mengembangkan kecerdasan secara holistik.</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="I27" s="4">
-        <v>0.85781370772764065</v>
+        <v>0.85780739795084104</v>
       </c>
       <c r="J27" s="4">
-        <v>0.95982878898857715</v>
+        <v>0.95983836263500533</v>
       </c>
       <c r="K27" s="4">
-        <v>0.75532643868539118</v>
+        <v>0.75529000760310905</v>
       </c>
       <c r="L27" s="7">
         <f t="shared" si="0"/>
-        <v>0.85765631180053636</v>
+        <v>0.85764525606298514</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -16147,26 +16213,26 @@
 Nama Direktur Pascasarjana Universitas Pendidikan Ganesha adalah Prof. Dr. I Nyoman Jampel, M.Pd.</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="I28" s="4">
-        <v>0.78456914454982929</v>
+        <v>0.7845826652918888</v>
       </c>
       <c r="J28" s="4">
-        <v>0.66501356164842729</v>
+        <v>0.66509526248292561</v>
       </c>
       <c r="K28" s="4">
-        <v>0.97547226004943743</v>
+        <v>0.97544721183929084</v>
       </c>
       <c r="L28" s="7">
         <f t="shared" si="0"/>
-        <v>0.80835165541589804</v>
+        <v>0.80837504653803505</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
@@ -16204,26 +16270,26 @@
 Jika Anda memerlukan informasi lebih lanjut mengenai masing-masing program, silakan tanyakan!</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="I29" s="4">
-        <v>0.91649039524868114</v>
+        <v>0.91648742633561253</v>
       </c>
       <c r="J29" s="4">
         <v>0.91964609785813023</v>
       </c>
       <c r="K29" s="4">
-        <v>0.73674206309274737</v>
+        <v>0.73677996486350894</v>
       </c>
       <c r="L29" s="7">
         <f t="shared" si="0"/>
-        <v>0.85762618539985291</v>
+        <v>0.85763782968575064</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
@@ -16245,26 +16311,26 @@
 Anda dapat mengakses informasi mengenai tata cara pembayaran Uang Kuliah Tunggal (UKT) mahasiswa baru Universitas Pendidikan Ganesha dengan layanan BRI Virtual Account (BRIVA) melalui link berikut: [Prosedur Pembayaran UKT Mahasiswa Baru Undiksha](https://undiksha.ac.id/prosedur-pembayaran-ukt-mahasiswa-baru-undiksha-dengan-layanan-bri-virtual-account-briva/).</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="I30" s="4">
-        <v>0.84575630741845753</v>
+        <v>0.84599509388948912</v>
       </c>
       <c r="J30" s="4">
-        <v>0.66993204839370368</v>
+        <v>0.67013920362622648</v>
       </c>
       <c r="K30" s="4">
-        <v>0.87856665978226467</v>
+        <v>0.87851167311059131</v>
       </c>
       <c r="L30" s="7">
         <f t="shared" si="0"/>
-        <v>0.79808500519814196</v>
+        <v>0.79821532354210234</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -16286,26 +16352,26 @@
 Informasi lebih lanjut mengenai prosedur pembayaran Uang Kuliah Tunggal (UKT) mahasiswa baru Universitas Pendidikan Ganesha dengan layanan BRI Virtual Account (BRIVA) dapat ditemukan di situs resmi Undiksha melalui tautan berikut: [Prosedur Pembayaran UKT Mahasiswa Baru Undiksha dengan Layanan BRI Virtual Account (BRIVA)](https://undiksha.ac.id/prosedur-pembayaran-ukt-mahasiswa-baru-undiksha-dengan-layanan-bri-virtual-account-briva/).</v>
       </c>
       <c r="F31" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="H31" s="5" t="s">
         <v>320</v>
       </c>
-      <c r="G31" s="5" t="s">
-        <v>321</v>
-      </c>
-      <c r="H31" s="5" t="s">
-        <v>323</v>
-      </c>
       <c r="I31" s="4">
-        <v>0.66510560574588196</v>
+        <v>0.66491587043603206</v>
       </c>
       <c r="J31" s="4">
-        <v>0.97497485074271706</v>
+        <v>0.9749838905250533</v>
       </c>
       <c r="K31" s="4">
-        <v>0.65486295297094688</v>
+        <v>0.65500305486725474</v>
       </c>
       <c r="L31" s="7">
         <f t="shared" si="0"/>
-        <v>0.76498113648651545</v>
+        <v>0.76496760527611352</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
@@ -16332,26 +16398,26 @@
 2. Lulusan Paket C tahun 2023, 2024, dan 2025 dengan umur maksimal 25 tahun (per 1 Juli 2025).</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="I32" s="4">
-        <v>0.86973210784034238</v>
+        <v>0.86970084039646911</v>
       </c>
       <c r="J32" s="4">
-        <v>0.98101976241736644</v>
+        <v>0.98103010719962414</v>
       </c>
       <c r="K32" s="4">
-        <v>0.94615459111656519</v>
+        <v>0.94614188609617189</v>
       </c>
       <c r="L32" s="7">
         <f t="shared" si="0"/>
-        <v>0.93230215379142456</v>
+        <v>0.93229094456408834</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
@@ -16392,26 +16458,26 @@
 Prinsip-prinsip ini bertujuan untuk menciptakan sistem seleksi yang berkualitas dan dapat dipercaya.</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="I33" s="4">
-        <v>0.77456111648330228</v>
+        <v>0.77462902245551502</v>
       </c>
       <c r="J33" s="4">
-        <v>0.88507532236005415</v>
+        <v>0.88495247459588366</v>
       </c>
       <c r="K33" s="4">
-        <v>0.85254522920003484</v>
+        <v>0.85254555289867917</v>
       </c>
       <c r="L33" s="7">
         <f t="shared" si="0"/>
-        <v>0.83739388934779713</v>
+        <v>0.83737568331669265</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
@@ -16433,26 +16499,26 @@
 Jadwal pendaftaran seleksi mahasiswa baru jalur mandiri (SMBJM) Universitas Pendidikan Ganesha untuk tahun 2025 akan diinformasikan segera. Untuk informasi lebih lanjut, Anda dapat mengunjungi situs resmi Undiksha atau mengikuti pengumuman resmi dari pihak universitas.</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="I34" s="4">
-        <v>0.84347750795950716</v>
+        <v>0.84349518702682236</v>
       </c>
       <c r="J34" s="4">
-        <v>1</v>
+        <v>0.99999905551293955</v>
       </c>
       <c r="K34" s="4">
-        <v>0.75900514735752123</v>
+        <v>0.75900877958117385</v>
       </c>
       <c r="L34" s="7">
         <f t="shared" si="0"/>
-        <v>0.86749421843900942</v>
+        <v>0.86750100737364522</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
@@ -16499,26 +16565,26 @@
 Jika ada pertanyaan lebih lanjut, silakan tanyakan!</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="H35" s="5" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="I35" s="4">
-        <v>0.99999904476278201</v>
+        <v>0.99999926840383169</v>
       </c>
       <c r="J35" s="4">
-        <v>0.88475391438539364</v>
+        <v>0.88742912767885429</v>
       </c>
       <c r="K35" s="4">
-        <v>0.88317727717427763</v>
+        <v>0.88309406612074937</v>
       </c>
       <c r="L35" s="7">
         <f t="shared" si="0"/>
-        <v>0.92264341210748446</v>
+        <v>0.92350748740114508</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
@@ -16554,26 +16620,26 @@
 5. Memenuhi persyaratan yang ditentukan oleh masing-masing PTN Akademik dan PTN Vokasi.</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="H36" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I36" s="4">
-        <v>0.93560893830652081</v>
+        <v>0.93561394505218931</v>
       </c>
       <c r="J36" s="4">
-        <v>0.9020573611359618</v>
+        <v>0.90207953861965084</v>
       </c>
       <c r="K36" s="4">
-        <v>0.99999906597946031</v>
+        <v>0.99999908303187324</v>
       </c>
       <c r="L36" s="7">
         <f t="shared" si="0"/>
-        <v>0.94588845514064757</v>
+        <v>0.94589752223457113</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
@@ -16612,26 +16678,26 @@
 Setiap tahapan UTBK-SNBT dibuka dan ditutup pada pukul 15.00 WIB.</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="H37" s="5" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="I37" s="4">
-        <v>1</v>
+        <v>0.999999143528572</v>
       </c>
       <c r="J37" s="4">
-        <v>0.84782102008685634</v>
+        <v>0.84780938193530198</v>
       </c>
       <c r="K37" s="4">
-        <v>0.89302678024758231</v>
+        <v>0.89299291595459485</v>
       </c>
       <c r="L37" s="7">
         <f t="shared" si="0"/>
-        <v>0.91361593344481296</v>
+        <v>0.91360048047282294</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
@@ -16653,26 +16719,26 @@
 Biaya untuk mengikuti Seleksi Nasional Berbasis Tes (SNBT) adalah sebesar Rp200.000,00 (dua ratus ribu rupiah). Pembayaran dilakukan melalui mitra bank yang ditentukan.</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="H38" s="5" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="I38" s="4">
-        <v>0.93232763100449978</v>
+        <v>0.932264779013386</v>
       </c>
       <c r="J38" s="4">
-        <v>0.97789626005626384</v>
+        <v>0.97792013715417281</v>
       </c>
       <c r="K38" s="4">
-        <v>0.90102664463049986</v>
+        <v>0.90105186894542921</v>
       </c>
       <c r="L38" s="7">
         <f t="shared" si="0"/>
-        <v>0.93708351189708783</v>
+        <v>0.93707892837099604</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
@@ -16709,26 +16775,26 @@
 Dengan demikian, UKM di Universitas Pendidikan Ganesha berkontribusi signifikan terhadap pengembangan diri mahasiswa di luar aspek akademik.</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="H39" s="5" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="I39" s="4">
-        <v>0.84738418350469835</v>
+        <v>0.84653118452727727</v>
       </c>
       <c r="J39" s="4">
-        <v>0.99014608638922041</v>
+        <v>0.99001139578688335</v>
       </c>
       <c r="K39" s="4">
-        <v>0.90001562247850631</v>
+        <v>0.89985423319977575</v>
       </c>
       <c r="L39" s="7">
         <f t="shared" si="0"/>
-        <v>0.91251529745747506</v>
+        <v>0.91213227117131213</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
@@ -16774,26 +16840,26 @@
 Dengan cara-cara di atas, Anda dapat memperoleh informasi yang Anda butuhkan mengenai UKM di Universitas Pendidikan Ganesha.</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="H40" s="5" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="I40" s="4">
-        <v>0.81304856453298602</v>
+        <v>0.81319408153592232</v>
       </c>
       <c r="J40" s="4">
-        <v>0.98987711145210378</v>
+        <v>0.99235910176147413</v>
       </c>
       <c r="K40" s="4">
-        <v>0.95661167999107344</v>
+        <v>0.95664915465655964</v>
       </c>
       <c r="L40" s="7">
         <f t="shared" si="0"/>
-        <v>0.91984578532538774</v>
+        <v>0.92073411265131877</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
@@ -16841,26 +16907,26 @@
 UPA TIK berfungsi untuk melaksanakan pengembangan, pengelolaan, dan pelayanan teknologi informasi dan komunikasi serta pengelolaan sistem informasi dan jaringan.</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="H41" s="5" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="I41" s="4">
-        <v>1</v>
+        <v>0.99999899983453544</v>
       </c>
       <c r="J41" s="4">
-        <v>0.87660142369597349</v>
+        <v>0.87665743069688673</v>
       </c>
       <c r="K41" s="4">
-        <v>0.83604400193260631</v>
+        <v>0.83615250120814411</v>
       </c>
       <c r="L41" s="7">
         <f t="shared" si="0"/>
-        <v>0.90421514187619323</v>
+        <v>0.90426964391318876</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
@@ -16882,26 +16948,26 @@
 Kepala UPA TIK Undiksha saat ini adalah I Ketut Resika Arthana, S.T., M.Kom.</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="H42" s="5" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="I42" s="4">
-        <v>0.88018924567650703</v>
+        <v>0.88035622762430632</v>
       </c>
       <c r="J42" s="4">
-        <v>0.85035886037065889</v>
+        <v>0.8502868521535073</v>
       </c>
       <c r="K42" s="4">
-        <v>0.79591931795592907</v>
+        <v>0.79590247782467005</v>
       </c>
       <c r="L42" s="7">
         <f t="shared" si="0"/>
-        <v>0.84215580800103174</v>
+        <v>0.84218185253416122</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
@@ -16923,26 +16989,26 @@
 Motto Universitas Pendidikan Ganesha (Undiksha) adalah “dharmaning sajjana umerdhyaken widyaguna” yang berarti kewajiban orang bijaksana adalah mengembangkan ilmu pengetahuan dan pekerti.</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="H43" s="5" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="I43" s="4">
-        <v>0.74649701138278635</v>
+        <v>0.74657379015409642</v>
       </c>
       <c r="J43" s="4">
-        <v>0.72420650675294918</v>
+        <v>0.72416558825096189</v>
       </c>
       <c r="K43" s="4">
-        <v>0.70140239285092598</v>
+        <v>0.69987205084048454</v>
       </c>
       <c r="L43" s="7">
         <f t="shared" si="0"/>
-        <v>0.72403530366222046</v>
+        <v>0.72353714308184769</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
@@ -16971,26 +17037,26 @@
 Dengan demikian, Undiksha menjadi satu-satunya perguruan tinggi negeri di Bali Utara yang memiliki akreditasi A dan diakui secara internasional.</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="H44" s="5" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="I44" s="4">
-        <v>0.99999882846985977</v>
+        <v>1</v>
       </c>
       <c r="J44" s="4">
-        <v>0.6206546840265279</v>
+        <v>0.62059982059192875</v>
       </c>
       <c r="K44" s="4">
-        <v>0.65259188610240804</v>
+        <v>0.65245297110805123</v>
       </c>
       <c r="L44" s="7">
         <f t="shared" si="0"/>
-        <v>0.75774846619959868</v>
+        <v>0.75768426389999333</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
@@ -17012,26 +17078,26 @@
 Visi Universitas Pendidikan Ganesha (Undiksha) adalah menjadi Universitas Unggul Berlandaskan Falsafah Tri Hita Karana di Asia Pada Tahun 2045. Visi ini mencerminkan komitmen Undiksha untuk mencapai keunggulan dengan mengedepankan nilai-nilai yang terkandung dalam falsafah Tri Hita Karana.</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="H45" s="5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="I45" s="4">
-        <v>0.72708997018892363</v>
+        <v>0.72719602964948771</v>
       </c>
       <c r="J45" s="4">
-        <v>0.85730713689993121</v>
+        <v>0.85721459525195143</v>
       </c>
       <c r="K45" s="4">
-        <v>0.99999897630410117</v>
+        <v>0.99999901834401395</v>
       </c>
       <c r="L45" s="7">
         <f t="shared" si="0"/>
-        <v>0.86146536113098537</v>
+        <v>0.86146988108181777</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
@@ -17053,26 +17119,26 @@
 Rektor Universitas Pendidikan Ganesha saat ini adalah Prof. Dr. I Wayan Lasmawan, M.Pd.</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="H46" s="5" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="I46" s="4">
-        <v>0.6801043957204197</v>
+        <v>0.67706695668706773</v>
       </c>
       <c r="J46" s="4">
-        <v>0.70305858091521545</v>
+        <v>0.70299784588680536</v>
       </c>
       <c r="K46" s="4">
-        <v>0.93774996628448071</v>
+        <v>0.93785812544872293</v>
       </c>
       <c r="L46" s="7">
         <f t="shared" si="0"/>
-        <v>0.77363764764003851</v>
+        <v>0.77264097600753201</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
@@ -17114,26 +17180,26 @@
 Selamat bergabung di Universitas Pendidikan Ganesha, KADEK YUNI SEDANI!</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="H47" s="5" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="I47" s="4">
-        <v>0.99999882693737174</v>
+        <v>0.99995130242305097</v>
       </c>
       <c r="J47" s="4">
-        <v>0.95135262994235947</v>
+        <v>0.95140876111475103</v>
       </c>
       <c r="K47" s="4">
-        <v>0.91865919494702064</v>
+        <v>0.9184090894366459</v>
       </c>
       <c r="L47" s="7">
         <f t="shared" si="0"/>
-        <v>0.95667021727558399</v>
+        <v>0.95658971765814937</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
@@ -17169,26 +17235,26 @@
 Silakan kirimkan informasi tersebut jika Anda memerlukan bantuan lebih lanjut.</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="H48" s="5" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="I48" s="4">
-        <v>0.86947361956584068</v>
+        <v>0.86950002028341766</v>
       </c>
       <c r="J48" s="4">
-        <v>0.96090498062395624</v>
+        <v>0.96093965710782059</v>
       </c>
       <c r="K48" s="4">
-        <v>0.81817813758246216</v>
+        <v>0.81825916600842885</v>
       </c>
       <c r="L48" s="7">
         <f t="shared" si="0"/>
-        <v>0.88285224592408651</v>
+        <v>0.88289961446655563</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
@@ -17218,26 +17284,26 @@
 Silakan klik tautan tersebut untuk mengunduh KTM Anda.</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="H49" s="5" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="I49" s="4">
-        <v>0.8243063373435856</v>
+        <v>0.82506620289957844</v>
       </c>
       <c r="J49" s="4">
-        <v>0.763940003192774</v>
+        <v>0.76738985489679434</v>
       </c>
       <c r="K49" s="4">
-        <v>0.77364783301889106</v>
+        <v>0.77871216182217384</v>
       </c>
       <c r="L49" s="7">
         <f t="shared" si="0"/>
-        <v>0.78729805785175022</v>
+        <v>0.79038940653951562</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
@@ -17274,26 +17340,26 @@
 Silakan kirimkan NIM Anda untuk mendapatkan informasi lebih lanjut.</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="H50" s="5" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="I50" s="4">
-        <v>0.99999925707396842</v>
+        <v>1</v>
       </c>
       <c r="J50" s="4">
-        <v>0.99343289137214108</v>
+        <v>0.99344415372452799</v>
       </c>
       <c r="K50" s="4">
-        <v>0.9934168034582046</v>
+        <v>0.99342618517590675</v>
       </c>
       <c r="L50" s="7">
         <f t="shared" si="0"/>
-        <v>0.99561631730143807</v>
+        <v>0.99562344630014488</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
@@ -17315,59 +17381,71 @@
 Pertanyaan tersebut tidak relevan dengan konteks kampus Universitas Pendidikan Ganesha.</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="H51" s="5" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="I51" s="4">
-        <v>0.3560510391217504</v>
+        <v>0.35614397789394242</v>
       </c>
       <c r="J51" s="4">
-        <v>0.83358117706137336</v>
+        <v>0.83361448543986238</v>
       </c>
       <c r="K51" s="4">
-        <v>0.24831459695925009</v>
+        <v>0.24823743264056891</v>
       </c>
       <c r="L51" s="7">
         <f t="shared" si="0"/>
-        <v>0.47931560438079135</v>
+        <v>0.47933196532479122</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A52" s="26"/>
-      <c r="B52" s="27"/>
-      <c r="C52" s="27"/>
-      <c r="D52" s="27"/>
-      <c r="E52" s="27"/>
-      <c r="F52" s="27"/>
-      <c r="G52" s="27"/>
-      <c r="H52" s="27"/>
-      <c r="I52" s="27"/>
-      <c r="J52" s="27"/>
-      <c r="K52" s="27"/>
-      <c r="L52" s="28"/>
+      <c r="A52" s="25"/>
+      <c r="B52" s="26"/>
+      <c r="C52" s="26"/>
+      <c r="D52" s="26"/>
+      <c r="E52" s="26"/>
+      <c r="F52" s="26"/>
+      <c r="G52" s="26"/>
+      <c r="H52" s="26"/>
+      <c r="I52" s="26"/>
+      <c r="J52" s="26"/>
+      <c r="K52" s="26"/>
+      <c r="L52" s="27"/>
     </row>
     <row r="53" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A53" s="29" t="s">
-        <v>230</v>
-      </c>
-      <c r="B53" s="30"/>
-      <c r="C53" s="30"/>
-      <c r="D53" s="30"/>
-      <c r="E53" s="30"/>
-      <c r="F53" s="30"/>
-      <c r="G53" s="30"/>
-      <c r="H53" s="30"/>
-      <c r="I53" s="30"/>
-      <c r="J53" s="30"/>
-      <c r="K53" s="31"/>
+      <c r="A53" s="28" t="s">
+        <v>227</v>
+      </c>
+      <c r="B53" s="29"/>
+      <c r="C53" s="29"/>
+      <c r="D53" s="29"/>
+      <c r="E53" s="29"/>
+      <c r="F53" s="29"/>
+      <c r="G53" s="29"/>
+      <c r="H53" s="29"/>
+      <c r="I53" s="29"/>
+      <c r="J53" s="29"/>
+      <c r="K53" s="30"/>
       <c r="L53" s="11">
         <f>IFERROR(AVERAGE(L2:L51),0)</f>
-        <v>0.85895356173206849</v>
+        <v>0.85901560927639264</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L56" s="17">
+        <f>MIN(L2:L51)</f>
+        <v>0.47933196532479122</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L57" s="17">
+        <f>MAX(L2:L51)</f>
+        <v>0.99562344630014488</v>
       </c>
     </row>
   </sheetData>
@@ -17383,9 +17461,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3728C640-F655-4ACE-93F4-7C1178A6920C}">
   <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17397,36 +17475,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="31" t="s">
+        <v>218</v>
+      </c>
+      <c r="B1" s="33" t="s">
+        <v>224</v>
+      </c>
+      <c r="C1" s="34"/>
+      <c r="D1" s="33" t="s">
+        <v>225</v>
+      </c>
+      <c r="E1" s="34"/>
+      <c r="F1" s="22" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="32"/>
+      <c r="B2" s="16" t="s">
+        <v>219</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>220</v>
+      </c>
+      <c r="D2" s="16" t="s">
         <v>221</v>
       </c>
-      <c r="B1" s="34" t="s">
-        <v>227</v>
-      </c>
-      <c r="C1" s="35"/>
-      <c r="D1" s="34" t="s">
-        <v>228</v>
-      </c>
-      <c r="E1" s="35"/>
-      <c r="F1" s="23" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="33"/>
-      <c r="B2" s="16" t="s">
+      <c r="E2" s="16" t="s">
         <v>222</v>
       </c>
-      <c r="C2" s="16" t="s">
-        <v>223</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>224</v>
-      </c>
-      <c r="E2" s="16" t="s">
-        <v>225</v>
-      </c>
-      <c r="F2" s="24"/>
+      <c r="F2" s="23"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
@@ -17446,11 +17524,11 @@
       </c>
       <c r="E3" s="15" cm="1">
         <f t="array" ref="E3:E52">IFERROR(RR!$L2:$L51,0)</f>
-        <v>0.76161836422559015</v>
+        <v>0.76170501431540105</v>
       </c>
       <c r="F3" s="15">
         <f>IFERROR(AVERAGE(B3:E3),0)</f>
-        <v>0.94040459105639751</v>
+        <v>0.94042625357885024</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -17467,11 +17545,11 @@
         <v>1</v>
       </c>
       <c r="E4" s="15">
-        <v>0.80981242725785707</v>
+        <v>0.80982548427416268</v>
       </c>
       <c r="F4" s="15">
         <f t="shared" ref="F4:F52" si="0">IFERROR(AVERAGE(B4:E4),0)</f>
-        <v>0.95245310681446427</v>
+        <v>0.95245637106854064</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -17488,11 +17566,11 @@
         <v>1</v>
       </c>
       <c r="E5" s="15">
-        <v>0.83514468342650094</v>
+        <v>0.83688674310992839</v>
       </c>
       <c r="F5" s="15">
         <f t="shared" si="0"/>
-        <v>0.95878617085662521</v>
+        <v>0.95922168577748212</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -17509,11 +17587,11 @@
         <v>1</v>
       </c>
       <c r="E6" s="15">
-        <v>0.86458597213040633</v>
+        <v>0.86440026625069288</v>
       </c>
       <c r="F6" s="15">
         <f t="shared" si="0"/>
-        <v>0.96614649303260158</v>
+        <v>0.96610006656267322</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -17530,11 +17608,11 @@
         <v>1</v>
       </c>
       <c r="E7" s="15">
-        <v>0.88465388518011823</v>
+        <v>0.88471054302820085</v>
       </c>
       <c r="F7" s="15">
         <f t="shared" si="0"/>
-        <v>0.97116347129502956</v>
+        <v>0.97117763575705018</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -17551,11 +17629,11 @@
         <v>1</v>
       </c>
       <c r="E8" s="15">
-        <v>0.75251901721403536</v>
+        <v>0.75253946345172784</v>
       </c>
       <c r="F8" s="15">
         <f t="shared" si="0"/>
-        <v>0.93812975430350887</v>
+        <v>0.93813486586293193</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -17572,11 +17650,11 @@
         <v>1</v>
       </c>
       <c r="E9" s="15">
-        <v>0.8866737706229525</v>
+        <v>0.88680199748219468</v>
       </c>
       <c r="F9" s="15">
         <f t="shared" si="0"/>
-        <v>0.97166844265573815</v>
+        <v>0.9717004993705487</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -17593,11 +17671,11 @@
         <v>1</v>
       </c>
       <c r="E10" s="15">
-        <v>0.80686434727441536</v>
+        <v>0.80687199784055386</v>
       </c>
       <c r="F10" s="15">
         <f t="shared" si="0"/>
-        <v>0.95171608681860387</v>
+        <v>0.95171799946013846</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -17614,11 +17692,11 @@
         <v>1</v>
       </c>
       <c r="E11" s="15">
-        <v>0.93993134247215782</v>
+        <v>0.93998011626732092</v>
       </c>
       <c r="F11" s="15">
         <f t="shared" si="0"/>
-        <v>0.98498283561803945</v>
+        <v>0.98499502906683023</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -17635,11 +17713,11 @@
         <v>1</v>
       </c>
       <c r="E12" s="15">
-        <v>0.93523266766798585</v>
+        <v>0.93525161069690499</v>
       </c>
       <c r="F12" s="15">
         <f t="shared" si="0"/>
-        <v>0.98380816691699646</v>
+        <v>0.98381290267422628</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -17656,11 +17734,11 @@
         <v>1</v>
       </c>
       <c r="E13" s="15">
-        <v>0.89212733483162632</v>
+        <v>0.89212951300674115</v>
       </c>
       <c r="F13" s="15">
         <f t="shared" si="0"/>
-        <v>0.97303183370790658</v>
+        <v>0.97303237825168531</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -17677,11 +17755,11 @@
         <v>1</v>
       </c>
       <c r="E14" s="15">
-        <v>0.84203095228593605</v>
+        <v>0.84189822952653703</v>
       </c>
       <c r="F14" s="15">
         <f t="shared" si="0"/>
-        <v>0.96050773807148404</v>
+        <v>0.96047455738163423</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -17698,11 +17776,11 @@
         <v>1</v>
       </c>
       <c r="E15" s="15">
-        <v>0.73663916821675501</v>
+        <v>0.73657402592247434</v>
       </c>
       <c r="F15" s="15">
         <f t="shared" si="0"/>
-        <v>0.93415979205418875</v>
+        <v>0.93414350648061861</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -17719,11 +17797,11 @@
         <v>1</v>
       </c>
       <c r="E16" s="15">
-        <v>0.88781938404459682</v>
+        <v>0.88771553966581873</v>
       </c>
       <c r="F16" s="15">
         <f t="shared" si="0"/>
-        <v>0.97195484601114923</v>
+        <v>0.97192888491645468</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -17740,11 +17818,11 @@
         <v>1</v>
       </c>
       <c r="E17" s="15">
-        <v>0.80737215410506724</v>
+        <v>0.80731691451692333</v>
       </c>
       <c r="F17" s="15">
         <f t="shared" si="0"/>
-        <v>0.95184303852626684</v>
+        <v>0.95182922862923081</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -17761,11 +17839,11 @@
         <v>1</v>
       </c>
       <c r="E18" s="15">
-        <v>0.92110747728249842</v>
+        <v>0.92109329220621516</v>
       </c>
       <c r="F18" s="15">
         <f t="shared" si="0"/>
-        <v>0.98027686932062463</v>
+        <v>0.98027332305155379</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -17782,11 +17860,11 @@
         <v>1</v>
       </c>
       <c r="E19" s="15">
-        <v>0.84240318019841531</v>
+        <v>0.84238246917305259</v>
       </c>
       <c r="F19" s="15">
         <f t="shared" si="0"/>
-        <v>0.96060079504960383</v>
+        <v>0.96059561729326315</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -17803,11 +17881,11 @@
         <v>1</v>
       </c>
       <c r="E20" s="15">
-        <v>0.90861149892977655</v>
+        <v>0.90858932692763583</v>
       </c>
       <c r="F20" s="15">
         <f t="shared" si="0"/>
-        <v>0.97715287473244417</v>
+        <v>0.97714733173190893</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -17824,11 +17902,11 @@
         <v>1</v>
       </c>
       <c r="E21" s="15">
-        <v>0.98393779246242963</v>
+        <v>0.98392905363163141</v>
       </c>
       <c r="F21" s="15">
         <f t="shared" si="0"/>
-        <v>0.99598444811560738</v>
+        <v>0.99598226340790785</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -17845,11 +17923,11 @@
         <v>1</v>
       </c>
       <c r="E22" s="15">
-        <v>0.90589808620165668</v>
+        <v>0.90590848904502597</v>
       </c>
       <c r="F22" s="15">
         <f t="shared" si="0"/>
-        <v>0.97647452155041414</v>
+        <v>0.97647712226125649</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -17866,11 +17944,11 @@
         <v>1</v>
       </c>
       <c r="E23" s="15">
-        <v>0.90722929012872067</v>
+        <v>0.9057018862402858</v>
       </c>
       <c r="F23" s="15">
         <f t="shared" si="0"/>
-        <v>0.97680732253218017</v>
+        <v>0.97642547156007142</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -17887,11 +17965,11 @@
         <v>1</v>
       </c>
       <c r="E24" s="15">
-        <v>0.88079742797158322</v>
+        <v>0.88081710646046896</v>
       </c>
       <c r="F24" s="15">
         <f t="shared" si="0"/>
-        <v>0.97019935699289583</v>
+        <v>0.97020427661511721</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -17908,11 +17986,11 @@
         <v>1</v>
       </c>
       <c r="E25" s="15">
-        <v>0.90398218744704073</v>
+        <v>0.90398912279127719</v>
       </c>
       <c r="F25" s="15">
         <f t="shared" si="0"/>
-        <v>0.97599554686176015</v>
+        <v>0.97599728069781932</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -17929,11 +18007,11 @@
         <v>1</v>
       </c>
       <c r="E26" s="15">
-        <v>0.91278270936526518</v>
+        <v>0.91277938856830299</v>
       </c>
       <c r="F26" s="15">
         <f t="shared" si="0"/>
-        <v>0.97819567734131629</v>
+        <v>0.97819484714207572</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -17950,11 +18028,11 @@
         <v>1</v>
       </c>
       <c r="E27" s="15">
-        <v>0.89740984316424888</v>
+        <v>0.89740545995089072</v>
       </c>
       <c r="F27" s="15">
         <f t="shared" si="0"/>
-        <v>0.97435246079106219</v>
+        <v>0.97435136498772268</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -17971,11 +18049,11 @@
         <v>1</v>
       </c>
       <c r="E28" s="15">
-        <v>0.85765631180053636</v>
+        <v>0.85764525606298514</v>
       </c>
       <c r="F28" s="15">
         <f t="shared" si="0"/>
-        <v>0.96441407795013412</v>
+        <v>0.96441131401574631</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -17992,11 +18070,11 @@
         <v>1</v>
       </c>
       <c r="E29" s="15">
-        <v>0.80835165541589804</v>
+        <v>0.80837504653803505</v>
       </c>
       <c r="F29" s="15">
         <f t="shared" si="0"/>
-        <v>0.95208791385397451</v>
+        <v>0.95209376163450876</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -18013,11 +18091,11 @@
         <v>1</v>
       </c>
       <c r="E30" s="15">
-        <v>0.85762618539985291</v>
+        <v>0.85763782968575064</v>
       </c>
       <c r="F30" s="15">
         <f t="shared" si="0"/>
-        <v>0.96440654634996326</v>
+        <v>0.96440945742143769</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -18034,11 +18112,11 @@
         <v>1</v>
       </c>
       <c r="E31" s="15">
-        <v>0.79808500519814196</v>
+        <v>0.79821532354210234</v>
       </c>
       <c r="F31" s="15">
         <f t="shared" si="0"/>
-        <v>0.94952125129953546</v>
+        <v>0.94955383088552558</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -18055,11 +18133,11 @@
         <v>1</v>
       </c>
       <c r="E32" s="15">
-        <v>0.76498113648651545</v>
+        <v>0.76496760527611352</v>
       </c>
       <c r="F32" s="15">
         <f t="shared" si="0"/>
-        <v>0.94124528412162889</v>
+        <v>0.94124190131902841</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -18076,11 +18154,11 @@
         <v>1</v>
       </c>
       <c r="E33" s="15">
-        <v>0.93230215379142456</v>
+        <v>0.93229094456408834</v>
       </c>
       <c r="F33" s="15">
         <f t="shared" si="0"/>
-        <v>0.98307553844785611</v>
+        <v>0.98307273614102209</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -18097,11 +18175,11 @@
         <v>1</v>
       </c>
       <c r="E34" s="15">
-        <v>0.83739388934779713</v>
+        <v>0.83737568331669265</v>
       </c>
       <c r="F34" s="15">
         <f t="shared" si="0"/>
-        <v>0.95934847233694931</v>
+        <v>0.95934392082917319</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -18118,11 +18196,11 @@
         <v>1</v>
       </c>
       <c r="E35" s="15">
-        <v>0.86749421843900942</v>
+        <v>0.86750100737364522</v>
       </c>
       <c r="F35" s="15">
         <f t="shared" si="0"/>
-        <v>0.96687355460975233</v>
+        <v>0.96687525184341128</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -18139,11 +18217,11 @@
         <v>1</v>
       </c>
       <c r="E36" s="15">
-        <v>0.92264341210748446</v>
+        <v>0.92350748740114508</v>
       </c>
       <c r="F36" s="15">
         <f t="shared" si="0"/>
-        <v>0.98066085302687112</v>
+        <v>0.98087687185028627</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -18160,11 +18238,11 @@
         <v>1</v>
       </c>
       <c r="E37" s="15">
-        <v>0.94588845514064757</v>
+        <v>0.94589752223457113</v>
       </c>
       <c r="F37" s="15">
         <f t="shared" si="0"/>
-        <v>0.98647211378516186</v>
+        <v>0.98647438055864278</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -18181,11 +18259,11 @@
         <v>1</v>
       </c>
       <c r="E38" s="15">
-        <v>0.91361593344481296</v>
+        <v>0.91360048047282294</v>
       </c>
       <c r="F38" s="15">
         <f t="shared" si="0"/>
-        <v>0.97840398336120327</v>
+        <v>0.97840012011820576</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -18202,11 +18280,11 @@
         <v>1</v>
       </c>
       <c r="E39" s="15">
-        <v>0.93708351189708783</v>
+        <v>0.93707892837099604</v>
       </c>
       <c r="F39" s="15">
         <f t="shared" si="0"/>
-        <v>0.98427087797427193</v>
+        <v>0.98426973209274904</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -18223,11 +18301,11 @@
         <v>1</v>
       </c>
       <c r="E40" s="15">
-        <v>0.91251529745747506</v>
+        <v>0.91213227117131213</v>
       </c>
       <c r="F40" s="15">
         <f t="shared" si="0"/>
-        <v>0.97812882436436877</v>
+        <v>0.97803306779282806</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -18244,11 +18322,11 @@
         <v>1</v>
       </c>
       <c r="E41" s="15">
-        <v>0.91984578532538774</v>
+        <v>0.92073411265131877</v>
       </c>
       <c r="F41" s="15">
         <f t="shared" si="0"/>
-        <v>0.97996144633134696</v>
+        <v>0.98018352816282972</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -18265,11 +18343,11 @@
         <v>1</v>
       </c>
       <c r="E42" s="15">
-        <v>0.90421514187619323</v>
+        <v>0.90426964391318876</v>
       </c>
       <c r="F42" s="15">
         <f t="shared" si="0"/>
-        <v>0.97605378546904831</v>
+        <v>0.97606741097829719</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -18286,11 +18364,11 @@
         <v>1</v>
       </c>
       <c r="E43" s="15">
-        <v>0.84215580800103174</v>
+        <v>0.84218185253416122</v>
       </c>
       <c r="F43" s="15">
         <f t="shared" si="0"/>
-        <v>0.96053895200025796</v>
+        <v>0.96054546313354028</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -18307,11 +18385,11 @@
         <v>1</v>
       </c>
       <c r="E44" s="15">
-        <v>0.72403530366222046</v>
+        <v>0.72353714308184769</v>
       </c>
       <c r="F44" s="15">
         <f t="shared" si="0"/>
-        <v>0.93100882591555512</v>
+        <v>0.93088428577046189</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -18328,11 +18406,11 @@
         <v>1</v>
       </c>
       <c r="E45" s="15">
-        <v>0.75774846619959868</v>
+        <v>0.75768426389999333</v>
       </c>
       <c r="F45" s="15">
         <f t="shared" si="0"/>
-        <v>0.9394371165498997</v>
+        <v>0.9394210659749983</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -18349,11 +18427,11 @@
         <v>1</v>
       </c>
       <c r="E46" s="15">
-        <v>0.86146536113098537</v>
+        <v>0.86146988108181777</v>
       </c>
       <c r="F46" s="15">
         <f t="shared" si="0"/>
-        <v>0.96536634028274637</v>
+        <v>0.96536747027045444</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -18370,11 +18448,11 @@
         <v>1</v>
       </c>
       <c r="E47" s="15">
-        <v>0.77363764764003851</v>
+        <v>0.77264097600753201</v>
       </c>
       <c r="F47" s="15">
         <f t="shared" si="0"/>
-        <v>0.9434094119100096</v>
+        <v>0.94316024400188303</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -18391,11 +18469,11 @@
         <v>0.875</v>
       </c>
       <c r="E48" s="15">
-        <v>0.95667021727558399</v>
+        <v>0.95658971765814937</v>
       </c>
       <c r="F48" s="15">
         <f t="shared" si="0"/>
-        <v>0.95791755431889603</v>
+        <v>0.95789742941453737</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -18412,11 +18490,11 @@
         <v>0.8</v>
       </c>
       <c r="E49" s="15">
-        <v>0.88285224592408651</v>
+        <v>0.88289961446655563</v>
       </c>
       <c r="F49" s="15">
         <f t="shared" si="0"/>
-        <v>0.92071306148102161</v>
+        <v>0.92072490361663883</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -18433,11 +18511,11 @@
         <v>0.75</v>
       </c>
       <c r="E50" s="15">
-        <v>0.78729805785175022</v>
+        <v>0.79038940653951562</v>
       </c>
       <c r="F50" s="15">
         <f t="shared" si="0"/>
-        <v>0.88432451446293758</v>
+        <v>0.8850973516348789</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -18454,11 +18532,11 @@
         <v>0.8</v>
       </c>
       <c r="E51" s="15">
-        <v>0.99561631730143807</v>
+        <v>0.99562344630014488</v>
       </c>
       <c r="F51" s="15">
         <f t="shared" si="0"/>
-        <v>0.94890407932535947</v>
+        <v>0.9489058615750362</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -18475,11 +18553,11 @@
         <v>1</v>
       </c>
       <c r="E52" s="15">
-        <v>0.47931560438079135</v>
+        <v>0.47933196532479122</v>
       </c>
       <c r="F52" s="15">
         <f t="shared" si="0"/>
-        <v>0.86982890109519784</v>
+        <v>0.86983299133119785</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -18490,9 +18568,9 @@
       <c r="E53" s="15"/>
       <c r="F53" s="15"/>
     </row>
-    <row r="54" spans="1:6" s="20" customFormat="1" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A54" s="21" t="s">
-        <v>229</v>
+    <row r="54" spans="1:6" s="19" customFormat="1" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A54" s="20" t="s">
+        <v>226</v>
       </c>
       <c r="B54" s="18">
         <f>IFERROR(AVERAGE(_xlfn.ANCHORARRAY($B$3)),0)</f>
@@ -18508,11 +18586,11 @@
       </c>
       <c r="E54" s="18">
         <f>IFERROR(AVERAGE(_xlfn.ANCHORARRAY($E$3)),0)</f>
-        <v>0.85895356173206849</v>
-      </c>
-      <c r="F54" s="19">
+        <v>0.85901560927639264</v>
+      </c>
+      <c r="F54" s="18">
         <f>IFERROR(AVERAGE(B54:E54),0)</f>
-        <v>0.96086339043301705</v>
+        <v>0.96087890231909812</v>
       </c>
     </row>
   </sheetData>
@@ -18549,38 +18627,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="22" t="s">
+      <c r="A1" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22" t="s">
+      <c r="C1" s="21"/>
+      <c r="D1" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="22"/>
-      <c r="F1" s="36" t="s">
-        <v>131</v>
-      </c>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="36" t="s">
+      <c r="E1" s="21"/>
+      <c r="F1" s="35" t="s">
+        <v>128</v>
+      </c>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="35" t="s">
+        <v>127</v>
+      </c>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="37"/>
+      <c r="O1" s="36"/>
+      <c r="P1" s="35" t="s">
         <v>130</v>
       </c>
-      <c r="L1" s="38"/>
-      <c r="M1" s="38"/>
-      <c r="N1" s="38"/>
-      <c r="O1" s="37"/>
-      <c r="P1" s="36" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q1" s="37"/>
+      <c r="Q1" s="36"/>
     </row>
     <row r="2" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="22"/>
+      <c r="A2" s="21"/>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
@@ -22138,43 +22216,43 @@
       </c>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A53" s="26"/>
-      <c r="B53" s="27"/>
-      <c r="C53" s="27"/>
-      <c r="D53" s="27"/>
-      <c r="E53" s="27"/>
-      <c r="F53" s="27"/>
-      <c r="G53" s="27"/>
-      <c r="H53" s="27"/>
-      <c r="I53" s="27"/>
-      <c r="J53" s="27"/>
-      <c r="K53" s="27"/>
-      <c r="L53" s="27"/>
-      <c r="M53" s="27"/>
-      <c r="N53" s="27"/>
-      <c r="O53" s="27"/>
-      <c r="P53" s="27"/>
-      <c r="Q53" s="28"/>
+      <c r="A53" s="25"/>
+      <c r="B53" s="26"/>
+      <c r="C53" s="26"/>
+      <c r="D53" s="26"/>
+      <c r="E53" s="26"/>
+      <c r="F53" s="26"/>
+      <c r="G53" s="26"/>
+      <c r="H53" s="26"/>
+      <c r="I53" s="26"/>
+      <c r="J53" s="26"/>
+      <c r="K53" s="26"/>
+      <c r="L53" s="26"/>
+      <c r="M53" s="26"/>
+      <c r="N53" s="26"/>
+      <c r="O53" s="26"/>
+      <c r="P53" s="26"/>
+      <c r="Q53" s="27"/>
     </row>
     <row r="54" spans="1:17" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A54" s="29" t="s">
-        <v>132</v>
-      </c>
-      <c r="B54" s="30"/>
-      <c r="C54" s="30"/>
-      <c r="D54" s="30"/>
-      <c r="E54" s="30"/>
-      <c r="F54" s="30"/>
-      <c r="G54" s="30"/>
-      <c r="H54" s="30"/>
-      <c r="I54" s="30"/>
-      <c r="J54" s="30"/>
-      <c r="K54" s="30"/>
-      <c r="L54" s="30"/>
-      <c r="M54" s="30"/>
-      <c r="N54" s="30"/>
-      <c r="O54" s="30"/>
-      <c r="P54" s="31"/>
+      <c r="A54" s="28" t="s">
+        <v>129</v>
+      </c>
+      <c r="B54" s="29"/>
+      <c r="C54" s="29"/>
+      <c r="D54" s="29"/>
+      <c r="E54" s="29"/>
+      <c r="F54" s="29"/>
+      <c r="G54" s="29"/>
+      <c r="H54" s="29"/>
+      <c r="I54" s="29"/>
+      <c r="J54" s="29"/>
+      <c r="K54" s="29"/>
+      <c r="L54" s="29"/>
+      <c r="M54" s="29"/>
+      <c r="N54" s="29"/>
+      <c r="O54" s="29"/>
+      <c r="P54" s="30"/>
       <c r="Q54" s="11">
         <f>IFERROR(AVERAGE(Q3:Q52),0)</f>
         <v>0</v>

</xml_diff>

<commit_message>
chore: update calc ragas
</commit_message>
<xml_diff>
--- a/test/human/calc/calc_testcase.xlsx
+++ b/test/human/calc/calc_testcase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Features\Documents\PMB-UNDIKSHA\va-pmb-undiksha\test\human\calc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA60C861-27BF-4112-9DDB-244D4B219B05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC7E655E-7B7D-45E9-B8D8-AEAFF329C98A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1AD30FE2-C1F0-4340-B4CE-7F2C452643D4}"/>
   </bookViews>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="407">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="401">
   <si>
     <t>No</t>
   </si>
@@ -182,19 +182,7 @@
     <t>Berikan informasi tentang Fakultas Bahasa dan Seni</t>
   </si>
   <si>
-    <t>Siapa nama Wakil Dekan I FE?</t>
-  </si>
-  <si>
-    <t>Visi Fakultas Ekonomi</t>
-  </si>
-  <si>
     <t>FHIS punya video profil?</t>
-  </si>
-  <si>
-    <t>Kapan FK didirikan?</t>
-  </si>
-  <si>
-    <t>Apa visi dari FMIPA?</t>
   </si>
   <si>
     <t>Pengembangan kurikulum Undiksha sesuai dengan apa?</t>
@@ -501,114 +489,12 @@
     <t>Berikan info mengenai Fakultas Bahasa dan Seni</t>
   </si>
   <si>
-    <t>Apa visi Fakultas Ekonomi?</t>
-  </si>
-  <si>
-    <t>Siapa nama Wakil Dekan Fakultas Ekonomi?</t>
-  </si>
-  <si>
-    <t>Nama Wakil Dekan FE</t>
-  </si>
-  <si>
-    <t>Visi yang dimiliki Fakultas Ekonomi</t>
-  </si>
-  <si>
-    <t>Informasi web FHIS</t>
-  </si>
-  <si>
-    <t>Apakah FHIS punya web?</t>
-  </si>
-  <si>
-    <t>Web FHIS Undiksha</t>
-  </si>
-  <si>
     <t>Apakah FHIS punya video profil?</t>
   </si>
   <si>
     <t>Video profil FHIS</t>
   </si>
   <si>
-    <t>Siapa nama dekan FIP Undiksha?</t>
-  </si>
-  <si>
-    <t>Nama dekan FIP</t>
-  </si>
-  <si>
-    <t>FIP nama dekannya siapa?</t>
-  </si>
-  <si>
-    <t>Kapan FIP mulai berdiri?</t>
-  </si>
-  <si>
-    <t>Kapan FIP mulai berdiri dengan jurusan yang awal?</t>
-  </si>
-  <si>
-    <t>Kapan FIP berdiri dan apa jurusan awalnya?</t>
-  </si>
-  <si>
-    <t>FK didirikan kapan?</t>
-  </si>
-  <si>
-    <t>Apa visi FK?</t>
-  </si>
-  <si>
-    <t>Apa visi yang dimiliki FK?</t>
-  </si>
-  <si>
-    <t>Visi dari FK</t>
-  </si>
-  <si>
-    <t>Apa visi yang dimiliki FMIPA?</t>
-  </si>
-  <si>
-    <t>Apa visi FMIPA?</t>
-  </si>
-  <si>
-    <t>Siapa nama dekan FMIPA?</t>
-  </si>
-  <si>
-    <t>Nama dekan FMIPA</t>
-  </si>
-  <si>
-    <t>Dekan FMIPA siapa?</t>
-  </si>
-  <si>
-    <t>Kapan program studi Pendidikan Olahraga dan Kesehatan berdiri di bawah Jurusan Pendidikan Matematika dan Ilmu Pengetahuan Alam (MIPA)?</t>
-  </si>
-  <si>
-    <t>Kapan Program Studi Pendidikan Olahraga dan Kesehatan pertama kali berdiri?</t>
-  </si>
-  <si>
-    <t>Kapan Program Studi Pendidikan Olahraga dan Kesehatan berdiri dan jurusan dibawahnya?</t>
-  </si>
-  <si>
-    <t>Apa visi FOK?</t>
-  </si>
-  <si>
-    <t>Visi dari FOK adalah</t>
-  </si>
-  <si>
-    <t>Sebutkan visi dari FOK!</t>
-  </si>
-  <si>
-    <t>Kapan FTK didirikan?</t>
-  </si>
-  <si>
-    <t>Kapan FTK berdiri dan program studi awal apa yang ditawarkan?</t>
-  </si>
-  <si>
-    <t>FTK kapan mulai berdiri? Dan apa program studi yang awal ditawarkan?</t>
-  </si>
-  <si>
-    <t>Siapa nama dekan FTK?</t>
-  </si>
-  <si>
-    <t>Nama dekan FTK</t>
-  </si>
-  <si>
-    <t>Dekan FTK siapa?</t>
-  </si>
-  <si>
     <t>Kurikulum Undiksha sesuai dengan apa?</t>
   </si>
   <si>
@@ -634,9 +520,6 @@
   </si>
   <si>
     <t>Ingin tau informasi cara mendapatkan layanan konseling di undiksha</t>
-  </si>
-  <si>
-    <t>Kapan Fakultas Kedokteran (FK) didirikan?</t>
   </si>
   <si>
     <t>Eg1</t>
@@ -3400,6 +3283,105 @@
 7. Beasiswa dari Pemda Bali (Dinas Pendidikan, Pemuda, dan Olahraga)
 8. Beasiswa Rektor Undiksha
 9. Beasiswa dari berbagai Pemda</t>
+  </si>
+  <si>
+    <t>Di mana saya dapat menemukan informasi lebih lanjut mengenai prosedur pembayaran UKT mahasiswa baru Universitas Pendidikan Ganesha?</t>
+  </si>
+  <si>
+    <t>Dimana informasi lebih lanjut mengenai prosedur pembayaran UKT dengan BRIVA?</t>
+  </si>
+  <si>
+    <t>Apa itu BRI Virtual Account (BRIVA) dan bagaimana cara menggunakannya untuk pembayaran UKT di Undiksha?</t>
+  </si>
+  <si>
+    <t>Kriteria peserta UTBK</t>
+  </si>
+  <si>
+    <t>Apa kriteria untuk peserta UTBK?</t>
+  </si>
+  <si>
+    <t>Apa saja kriteria peserta untuk bisa mengikuti UTBK?</t>
+  </si>
+  <si>
+    <t>Kapan jadwal pendaftaran untuk SMBJM undiksha dibuka?</t>
+  </si>
+  <si>
+    <t>Jadwal SMBJM</t>
+  </si>
+  <si>
+    <t>Kapan pelaksanaan SNBP?</t>
+  </si>
+  <si>
+    <t>Jadwal SNBP</t>
+  </si>
+  <si>
+    <t>Apa syarat mendaftar SNBP?</t>
+  </si>
+  <si>
+    <t>Syarat bagi siswa yang ingin mendaftar SNBP</t>
+  </si>
+  <si>
+    <t>Kapan pelaksanaan SNBT?</t>
+  </si>
+  <si>
+    <t>Jadwal SNBT</t>
+  </si>
+  <si>
+    <t>Berapa biaya mengikuti Tes SNBT?</t>
+  </si>
+  <si>
+    <t>Berapa biaya yang diperlukan untuk mengikuti SNBT?</t>
+  </si>
+  <si>
+    <t>Biaya untuk mengikuti SNBT</t>
+  </si>
+  <si>
+    <t>Apa fungsi utama UKM?</t>
+  </si>
+  <si>
+    <t>Apa fungsi utama dari UKM di Universitas Pendidikan Ganesha?</t>
+  </si>
+  <si>
+    <t>Fungsi utama UKM di Universitas Pendidikan Ganesha</t>
+  </si>
+  <si>
+    <t>Bagaimana cara mendapatkan informasi mengenai UKM di Universitas Pendidikan Ganesha?</t>
+  </si>
+  <si>
+    <t>Bagaimana cara mendapat informasi lebih lanjut mengenai UKM di Undiksha?</t>
+  </si>
+  <si>
+    <t>Apa langkah-langkah untuk mendapat informasi lebih lanjut tentang UKM di Undiksha?</t>
+  </si>
+  <si>
+    <t>Apa motto Undiksha?</t>
+  </si>
+  <si>
+    <t>Motto yang dimiliki undiksha?</t>
+  </si>
+  <si>
+    <t>Sebutkan motto yang dimiliki Undiksha!</t>
+  </si>
+  <si>
+    <t>Undiksha memiliki akreditasi apa saja?</t>
+  </si>
+  <si>
+    <t>Akreditasi apa yang dimiliki undiksha?</t>
+  </si>
+  <si>
+    <t>Apa visi Undiksha?</t>
+  </si>
+  <si>
+    <t>Visi Universitas Pendidikan Ganesha apa?</t>
+  </si>
+  <si>
+    <t>Siapa rektor undiksha?</t>
+  </si>
+  <si>
+    <t>Siapa nama rektor Undiksha?</t>
+  </si>
+  <si>
+    <t>Siapa rektor Universitas Pendidikan Ganesha?</t>
   </si>
 </sst>
 </file>
@@ -4558,7 +4540,7 @@
                   <c:v>0.92195604395604402</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.86828812217401496</c:v>
+                  <c:v>0.8596862674719985</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5938,79 +5920,79 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="25"/>
                 <c:pt idx="0">
-                  <c:v>0.76170501431540105</c:v>
+                  <c:v>0.76170980330341098</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.80982548427416268</c:v>
+                  <c:v>0.80974497289702896</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.83688674310992839</c:v>
+                  <c:v>0.83517786398888127</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.86440026625069288</c:v>
+                  <c:v>0.86448749635843181</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.88471054302820085</c:v>
+                  <c:v>0.88483143960560495</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.75253946345172784</c:v>
+                  <c:v>0.7516873559080679</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.88680199748219468</c:v>
+                  <c:v>0.88666271689387044</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.80687199784055386</c:v>
+                  <c:v>0.80693257905267401</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.93998011626732092</c:v>
+                  <c:v>0.93992850487830337</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.93525161069690499</c:v>
+                  <c:v>0.93511326350330537</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.89212951300674115</c:v>
+                  <c:v>0.88775978840688852</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.84189822952653703</c:v>
+                  <c:v>0.89729636971955451</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.73657402592247434</c:v>
+                  <c:v>0.76495019792620411</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.88771553966581873</c:v>
+                  <c:v>0.93228634374802377</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.80731691451692333</c:v>
+                  <c:v>0.86753442343354903</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.92109329220621516</c:v>
+                  <c:v>0.92350451372721454</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.84238246917305259</c:v>
+                  <c:v>0.9459137754961322</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.90858932692763583</c:v>
+                  <c:v>0.91358604714253155</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.98392905363163141</c:v>
+                  <c:v>0.93708099560022939</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.90590848904502597</c:v>
+                  <c:v>0.91251092088588548</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.9057018862402858</c:v>
+                  <c:v>0.91990366860756589</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.88081710646046896</c:v>
+                  <c:v>0.72399592513498712</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.90398912279127719</c:v>
+                  <c:v>0.75560027350827319</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.91277938856830299</c:v>
+                  <c:v>0.8614733586432336</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.89740545995089072</c:v>
+                  <c:v>0.77248408843010463</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10087,8 +10069,8 @@
   <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
+      <pane ySplit="2" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10120,7 +10102,7 @@
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>2</v>
@@ -10134,13 +10116,13 @@
         <v>29</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>406</v>
+        <v>367</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>170</v>
+        <v>131</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>171</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="12" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
@@ -10151,13 +10133,13 @@
         <v>30</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>172</v>
+        <v>133</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>173</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="12" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
@@ -10168,13 +10150,13 @@
         <v>31</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>174</v>
+        <v>135</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>175</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="12" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
@@ -10185,13 +10167,13 @@
         <v>32</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>176</v>
+        <v>137</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>177</v>
+        <v>138</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="12" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
@@ -10202,13 +10184,13 @@
         <v>33</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>178</v>
+        <v>139</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="12" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
@@ -10219,13 +10201,13 @@
         <v>34</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>179</v>
+        <v>140</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>180</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="12" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
@@ -10236,13 +10218,13 @@
         <v>35</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>181</v>
+        <v>142</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>182</v>
+        <v>143</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>183</v>
+        <v>144</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="12" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
@@ -10253,13 +10235,13 @@
         <v>36</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>184</v>
+        <v>145</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>185</v>
+        <v>146</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="12" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
@@ -10270,13 +10252,13 @@
         <v>37</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>186</v>
+        <v>147</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:5" s="12" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
@@ -10287,13 +10269,13 @@
         <v>38</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>187</v>
+        <v>148</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>188</v>
+        <v>149</v>
       </c>
     </row>
     <row r="13" spans="1:5" s="12" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
@@ -10301,16 +10283,16 @@
         <v>11</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>189</v>
+        <v>150</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:5" s="12" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
@@ -10318,16 +10300,16 @@
         <v>12</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>190</v>
+        <v>151</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>191</v>
+        <v>152</v>
       </c>
     </row>
     <row r="15" spans="1:5" s="12" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
@@ -10335,16 +10317,16 @@
         <v>13</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>192</v>
+        <v>153</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>193</v>
+        <v>154</v>
       </c>
     </row>
     <row r="16" spans="1:5" s="12" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
@@ -10352,16 +10334,16 @@
         <v>14</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>194</v>
+        <v>155</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>195</v>
+        <v>156</v>
       </c>
     </row>
     <row r="17" spans="1:5" s="12" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
@@ -10369,16 +10351,16 @@
         <v>15</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>196</v>
+        <v>157</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>197</v>
+        <v>158</v>
       </c>
     </row>
     <row r="18" spans="1:5" s="12" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
@@ -10386,16 +10368,16 @@
         <v>16</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>198</v>
+        <v>159</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>199</v>
+        <v>160</v>
       </c>
     </row>
     <row r="19" spans="1:5" s="12" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
@@ -10403,16 +10385,16 @@
         <v>17</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>200</v>
+        <v>161</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:5" s="12" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
@@ -10420,16 +10402,16 @@
         <v>18</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>201</v>
+        <v>162</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>202</v>
+        <v>163</v>
       </c>
     </row>
     <row r="21" spans="1:5" s="12" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
@@ -10437,16 +10419,16 @@
         <v>19</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>203</v>
+        <v>164</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>204</v>
+        <v>165</v>
       </c>
     </row>
     <row r="22" spans="1:5" s="12" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
@@ -10454,16 +10436,16 @@
         <v>20</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>205</v>
+        <v>166</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>206</v>
+        <v>167</v>
       </c>
     </row>
     <row r="23" spans="1:5" s="12" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
@@ -10471,16 +10453,16 @@
         <v>21</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>207</v>
+        <v>168</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>208</v>
+        <v>169</v>
       </c>
     </row>
     <row r="24" spans="1:5" s="12" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
@@ -10488,16 +10470,16 @@
         <v>22</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>209</v>
+        <v>170</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25" spans="1:5" s="12" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
@@ -10505,16 +10487,16 @@
         <v>23</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>210</v>
+        <v>171</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:5" s="12" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
@@ -10522,16 +10504,16 @@
         <v>24</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>211</v>
+        <v>172</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="27" spans="1:5" s="12" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
@@ -10539,16 +10521,16 @@
         <v>25</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>212</v>
+        <v>173</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -10583,7 +10565,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="21" t="s">
-        <v>214</v>
+        <v>175</v>
       </c>
       <c r="C1" s="21" t="s">
         <v>26</v>
@@ -10595,70 +10577,70 @@
         <v>28</v>
       </c>
       <c r="F1" s="21" t="s">
-        <v>215</v>
+        <v>176</v>
       </c>
       <c r="G1" s="21" t="s">
-        <v>216</v>
+        <v>177</v>
       </c>
       <c r="H1" s="21" t="s">
-        <v>217</v>
+        <v>178</v>
       </c>
       <c r="I1" s="21" t="s">
-        <v>218</v>
+        <v>179</v>
       </c>
       <c r="J1" s="21" t="s">
-        <v>219</v>
+        <v>180</v>
       </c>
       <c r="K1" s="21" t="s">
-        <v>220</v>
+        <v>181</v>
       </c>
       <c r="L1" s="21" t="s">
-        <v>221</v>
+        <v>182</v>
       </c>
       <c r="M1" s="21" t="s">
-        <v>222</v>
+        <v>183</v>
       </c>
       <c r="N1" s="21" t="s">
-        <v>223</v>
+        <v>184</v>
       </c>
       <c r="O1" s="21" t="s">
-        <v>224</v>
+        <v>185</v>
       </c>
       <c r="P1" s="21" t="s">
-        <v>225</v>
+        <v>186</v>
       </c>
       <c r="Q1" s="21" t="s">
-        <v>226</v>
+        <v>187</v>
       </c>
       <c r="R1" s="21" t="s">
-        <v>227</v>
+        <v>188</v>
       </c>
       <c r="S1" s="21" t="s">
-        <v>228</v>
+        <v>189</v>
       </c>
       <c r="T1" s="21" t="s">
-        <v>229</v>
+        <v>190</v>
       </c>
       <c r="U1" s="21" t="s">
-        <v>230</v>
+        <v>191</v>
       </c>
       <c r="V1" s="21" t="s">
-        <v>231</v>
+        <v>192</v>
       </c>
       <c r="W1" s="21" t="s">
-        <v>232</v>
+        <v>193</v>
       </c>
       <c r="X1" s="21" t="s">
-        <v>233</v>
+        <v>194</v>
       </c>
       <c r="Y1" s="21" t="s">
-        <v>234</v>
+        <v>195</v>
       </c>
       <c r="Z1" s="21" t="s">
-        <v>235</v>
+        <v>196</v>
       </c>
       <c r="AA1" s="21" t="s">
-        <v>236</v>
+        <v>197</v>
       </c>
     </row>
     <row r="2" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
@@ -10666,7 +10648,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>237</v>
+        <v>198</v>
       </c>
       <c r="C2" s="24">
         <v>0</v>
@@ -10749,7 +10731,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>238</v>
+        <v>199</v>
       </c>
       <c r="C3" s="24">
         <v>0</v>
@@ -10832,7 +10814,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>239</v>
+        <v>200</v>
       </c>
       <c r="C4" s="24">
         <v>0</v>
@@ -10915,7 +10897,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>240</v>
+        <v>201</v>
       </c>
       <c r="C5" s="24">
         <v>0</v>
@@ -10998,7 +10980,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>241</v>
+        <v>202</v>
       </c>
       <c r="C6" s="24">
         <v>0</v>
@@ -11081,7 +11063,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>242</v>
+        <v>203</v>
       </c>
       <c r="C7" s="24">
         <v>0</v>
@@ -11164,7 +11146,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>243</v>
+        <v>204</v>
       </c>
       <c r="C8" s="24">
         <v>0</v>
@@ -11247,7 +11229,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>244</v>
+        <v>205</v>
       </c>
       <c r="C9" s="24">
         <v>0</v>
@@ -11330,7 +11312,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>245</v>
+        <v>206</v>
       </c>
       <c r="C10" s="24">
         <v>0</v>
@@ -11413,7 +11395,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>246</v>
+        <v>207</v>
       </c>
       <c r="C11" s="24">
         <v>0</v>
@@ -11496,7 +11478,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>247</v>
+        <v>208</v>
       </c>
       <c r="C12" s="24">
         <v>0</v>
@@ -11579,7 +11561,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>248</v>
+        <v>209</v>
       </c>
       <c r="C13" s="24">
         <v>0</v>
@@ -11662,7 +11644,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>249</v>
+        <v>210</v>
       </c>
       <c r="C14" s="24">
         <v>0</v>
@@ -11745,7 +11727,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>250</v>
+        <v>211</v>
       </c>
       <c r="C15" s="24">
         <v>0</v>
@@ -11828,7 +11810,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="23" t="s">
-        <v>251</v>
+        <v>212</v>
       </c>
       <c r="C16" s="24">
         <v>0</v>
@@ -11911,7 +11893,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>252</v>
+        <v>213</v>
       </c>
       <c r="C17" s="24">
         <v>0</v>
@@ -11994,7 +11976,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="23" t="s">
-        <v>253</v>
+        <v>214</v>
       </c>
       <c r="C18" s="24">
         <v>0</v>
@@ -12077,7 +12059,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="23" t="s">
-        <v>254</v>
+        <v>215</v>
       </c>
       <c r="C19" s="24">
         <v>0</v>
@@ -12160,7 +12142,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="23" t="s">
-        <v>255</v>
+        <v>216</v>
       </c>
       <c r="C20" s="24">
         <v>0</v>
@@ -12243,7 +12225,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="23" t="s">
-        <v>256</v>
+        <v>217</v>
       </c>
       <c r="C21" s="24">
         <v>0</v>
@@ -12326,7 +12308,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="23" t="s">
-        <v>257</v>
+        <v>218</v>
       </c>
       <c r="C22" s="24">
         <v>0</v>
@@ -12409,7 +12391,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>258</v>
+        <v>219</v>
       </c>
       <c r="C23" s="24">
         <v>0</v>
@@ -12492,7 +12474,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="23" t="s">
-        <v>259</v>
+        <v>220</v>
       </c>
       <c r="C24" s="24">
         <v>0</v>
@@ -12575,7 +12557,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="23" t="s">
-        <v>260</v>
+        <v>221</v>
       </c>
       <c r="C25" s="24">
         <v>0</v>
@@ -12658,7 +12640,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="23" t="s">
-        <v>261</v>
+        <v>222</v>
       </c>
       <c r="C26" s="24">
         <v>0</v>
@@ -12741,7 +12723,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="23" t="s">
-        <v>262</v>
+        <v>223</v>
       </c>
       <c r="C27" s="24">
         <v>0</v>
@@ -12824,7 +12806,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="23" t="s">
-        <v>263</v>
+        <v>224</v>
       </c>
       <c r="C28" s="24">
         <v>0</v>
@@ -12907,7 +12889,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="23" t="s">
-        <v>264</v>
+        <v>225</v>
       </c>
       <c r="C29" s="24">
         <v>0</v>
@@ -12990,7 +12972,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="23" t="s">
-        <v>265</v>
+        <v>226</v>
       </c>
       <c r="C30" s="24">
         <v>0</v>
@@ -13073,7 +13055,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="23" t="s">
-        <v>266</v>
+        <v>227</v>
       </c>
       <c r="C31" s="24">
         <v>1</v>
@@ -13156,7 +13138,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="23" t="s">
-        <v>267</v>
+        <v>228</v>
       </c>
       <c r="C32" s="24">
         <v>0</v>
@@ -13239,7 +13221,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="23" t="s">
-        <v>268</v>
+        <v>229</v>
       </c>
       <c r="C33" s="24">
         <v>0</v>
@@ -13322,7 +13304,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="23" t="s">
-        <v>269</v>
+        <v>230</v>
       </c>
       <c r="C34" s="24">
         <v>0</v>
@@ -13405,7 +13387,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="23" t="s">
-        <v>270</v>
+        <v>231</v>
       </c>
       <c r="C35" s="24">
         <v>0</v>
@@ -13488,7 +13470,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="23" t="s">
-        <v>271</v>
+        <v>232</v>
       </c>
       <c r="C36" s="24">
         <v>0</v>
@@ -13571,7 +13553,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="23" t="s">
-        <v>272</v>
+        <v>233</v>
       </c>
       <c r="C37" s="24">
         <v>0</v>
@@ -13654,7 +13636,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="23" t="s">
-        <v>273</v>
+        <v>234</v>
       </c>
       <c r="C38" s="24">
         <v>0</v>
@@ -13737,7 +13719,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="23" t="s">
-        <v>274</v>
+        <v>235</v>
       </c>
       <c r="C39" s="24">
         <v>0</v>
@@ -13820,7 +13802,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="23" t="s">
-        <v>275</v>
+        <v>236</v>
       </c>
       <c r="C40" s="24">
         <v>0</v>
@@ -13903,7 +13885,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="23" t="s">
-        <v>276</v>
+        <v>237</v>
       </c>
       <c r="C41" s="24">
         <v>0</v>
@@ -13986,7 +13968,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="23" t="s">
-        <v>277</v>
+        <v>238</v>
       </c>
       <c r="C42" s="24">
         <v>0</v>
@@ -14069,7 +14051,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="23" t="s">
-        <v>278</v>
+        <v>239</v>
       </c>
       <c r="C43" s="24">
         <v>0</v>
@@ -14152,7 +14134,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="23" t="s">
-        <v>279</v>
+        <v>240</v>
       </c>
       <c r="C44" s="24">
         <v>0</v>
@@ -14235,7 +14217,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="23" t="s">
-        <v>280</v>
+        <v>241</v>
       </c>
       <c r="C45" s="24">
         <v>0</v>
@@ -14318,7 +14300,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="23" t="s">
-        <v>281</v>
+        <v>242</v>
       </c>
       <c r="C46" s="24">
         <v>0</v>
@@ -14401,7 +14383,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="23" t="s">
-        <v>282</v>
+        <v>243</v>
       </c>
       <c r="C47" s="24">
         <v>0</v>
@@ -14484,7 +14466,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="23" t="s">
-        <v>283</v>
+        <v>244</v>
       </c>
       <c r="C48" s="24">
         <v>0</v>
@@ -14567,7 +14549,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="23" t="s">
-        <v>284</v>
+        <v>245</v>
       </c>
       <c r="C49" s="24">
         <v>0</v>
@@ -14650,7 +14632,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="23" t="s">
-        <v>285</v>
+        <v>246</v>
       </c>
       <c r="C50" s="24">
         <v>0</v>
@@ -14733,7 +14715,7 @@
         <v>50</v>
       </c>
       <c r="B51" s="23" t="s">
-        <v>286</v>
+        <v>247</v>
       </c>
       <c r="C51" s="24">
         <v>0</v>
@@ -14816,7 +14798,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="23" t="s">
-        <v>287</v>
+        <v>248</v>
       </c>
       <c r="C52" s="24">
         <v>0</v>
@@ -14899,7 +14881,7 @@
         <v>52</v>
       </c>
       <c r="B53" s="23" t="s">
-        <v>288</v>
+        <v>249</v>
       </c>
       <c r="C53" s="24">
         <v>0</v>
@@ -14982,7 +14964,7 @@
         <v>53</v>
       </c>
       <c r="B54" s="23" t="s">
-        <v>289</v>
+        <v>250</v>
       </c>
       <c r="C54" s="24">
         <v>0</v>
@@ -15065,7 +15047,7 @@
         <v>54</v>
       </c>
       <c r="B55" s="23" t="s">
-        <v>290</v>
+        <v>251</v>
       </c>
       <c r="C55" s="24">
         <v>0</v>
@@ -15148,7 +15130,7 @@
         <v>55</v>
       </c>
       <c r="B56" s="23" t="s">
-        <v>291</v>
+        <v>252</v>
       </c>
       <c r="C56" s="24">
         <v>0</v>
@@ -15231,7 +15213,7 @@
         <v>56</v>
       </c>
       <c r="B57" s="23" t="s">
-        <v>292</v>
+        <v>253</v>
       </c>
       <c r="C57" s="24">
         <v>0</v>
@@ -15314,7 +15296,7 @@
         <v>57</v>
       </c>
       <c r="B58" s="23" t="s">
-        <v>293</v>
+        <v>254</v>
       </c>
       <c r="C58" s="24">
         <v>0</v>
@@ -15397,7 +15379,7 @@
         <v>58</v>
       </c>
       <c r="B59" s="23" t="s">
-        <v>294</v>
+        <v>255</v>
       </c>
       <c r="C59" s="24">
         <v>0</v>
@@ -15480,7 +15462,7 @@
         <v>59</v>
       </c>
       <c r="B60" s="23" t="s">
-        <v>295</v>
+        <v>256</v>
       </c>
       <c r="C60" s="24">
         <v>0</v>
@@ -15563,7 +15545,7 @@
         <v>60</v>
       </c>
       <c r="B61" s="23" t="s">
-        <v>296</v>
+        <v>257</v>
       </c>
       <c r="C61" s="24">
         <v>0</v>
@@ -15646,7 +15628,7 @@
         <v>61</v>
       </c>
       <c r="B62" s="23" t="s">
-        <v>297</v>
+        <v>258</v>
       </c>
       <c r="C62" s="24">
         <v>0</v>
@@ -15729,7 +15711,7 @@
         <v>62</v>
       </c>
       <c r="B63" s="23" t="s">
-        <v>298</v>
+        <v>259</v>
       </c>
       <c r="C63" s="24">
         <v>0</v>
@@ -15812,7 +15794,7 @@
         <v>63</v>
       </c>
       <c r="B64" s="23" t="s">
-        <v>299</v>
+        <v>260</v>
       </c>
       <c r="C64" s="24">
         <v>0</v>
@@ -15895,7 +15877,7 @@
         <v>64</v>
       </c>
       <c r="B65" s="23" t="s">
-        <v>300</v>
+        <v>261</v>
       </c>
       <c r="C65" s="24">
         <v>0</v>
@@ -15978,7 +15960,7 @@
         <v>65</v>
       </c>
       <c r="B66" s="23" t="s">
-        <v>301</v>
+        <v>262</v>
       </c>
       <c r="C66" s="24">
         <v>0</v>
@@ -16061,7 +16043,7 @@
         <v>66</v>
       </c>
       <c r="B67" s="23" t="s">
-        <v>302</v>
+        <v>263</v>
       </c>
       <c r="C67" s="24">
         <v>0</v>
@@ -16144,7 +16126,7 @@
         <v>67</v>
       </c>
       <c r="B68" s="23" t="s">
-        <v>303</v>
+        <v>264</v>
       </c>
       <c r="C68" s="24">
         <v>0</v>
@@ -16227,7 +16209,7 @@
         <v>68</v>
       </c>
       <c r="B69" s="23" t="s">
-        <v>304</v>
+        <v>265</v>
       </c>
       <c r="C69" s="24">
         <v>0</v>
@@ -16310,7 +16292,7 @@
         <v>69</v>
       </c>
       <c r="B70" s="23" t="s">
-        <v>305</v>
+        <v>266</v>
       </c>
       <c r="C70" s="24">
         <v>0</v>
@@ -16393,7 +16375,7 @@
         <v>70</v>
       </c>
       <c r="B71" s="23" t="s">
-        <v>306</v>
+        <v>267</v>
       </c>
       <c r="C71" s="24">
         <v>0</v>
@@ -16476,7 +16458,7 @@
         <v>71</v>
       </c>
       <c r="B72" s="23" t="s">
-        <v>307</v>
+        <v>268</v>
       </c>
       <c r="C72" s="24">
         <v>0</v>
@@ -16559,7 +16541,7 @@
         <v>72</v>
       </c>
       <c r="B73" s="23" t="s">
-        <v>308</v>
+        <v>269</v>
       </c>
       <c r="C73" s="24">
         <v>0</v>
@@ -16642,7 +16624,7 @@
         <v>73</v>
       </c>
       <c r="B74" s="23" t="s">
-        <v>309</v>
+        <v>270</v>
       </c>
       <c r="C74" s="24">
         <v>0</v>
@@ -16725,7 +16707,7 @@
         <v>74</v>
       </c>
       <c r="B75" s="23" t="s">
-        <v>310</v>
+        <v>271</v>
       </c>
       <c r="C75" s="24">
         <v>0</v>
@@ -16808,7 +16790,7 @@
         <v>75</v>
       </c>
       <c r="B76" s="23" t="s">
-        <v>311</v>
+        <v>272</v>
       </c>
       <c r="C76" s="24">
         <v>1</v>
@@ -16891,7 +16873,7 @@
         <v>76</v>
       </c>
       <c r="B77" s="23" t="s">
-        <v>312</v>
+        <v>273</v>
       </c>
       <c r="C77" s="24">
         <v>0</v>
@@ -16974,7 +16956,7 @@
         <v>77</v>
       </c>
       <c r="B78" s="23" t="s">
-        <v>313</v>
+        <v>274</v>
       </c>
       <c r="C78" s="24">
         <v>0</v>
@@ -17057,7 +17039,7 @@
         <v>78</v>
       </c>
       <c r="B79" s="23" t="s">
-        <v>314</v>
+        <v>275</v>
       </c>
       <c r="C79" s="24">
         <v>0</v>
@@ -17140,7 +17122,7 @@
         <v>79</v>
       </c>
       <c r="B80" s="23" t="s">
-        <v>315</v>
+        <v>276</v>
       </c>
       <c r="C80" s="24">
         <v>0</v>
@@ -17223,7 +17205,7 @@
         <v>80</v>
       </c>
       <c r="B81" s="23" t="s">
-        <v>316</v>
+        <v>277</v>
       </c>
       <c r="C81" s="24">
         <v>0</v>
@@ -17306,7 +17288,7 @@
         <v>81</v>
       </c>
       <c r="B82" s="23" t="s">
-        <v>317</v>
+        <v>278</v>
       </c>
       <c r="C82" s="24">
         <v>0</v>
@@ -17389,7 +17371,7 @@
         <v>82</v>
       </c>
       <c r="B83" s="23" t="s">
-        <v>318</v>
+        <v>279</v>
       </c>
       <c r="C83" s="24">
         <v>0</v>
@@ -17472,7 +17454,7 @@
         <v>83</v>
       </c>
       <c r="B84" s="23" t="s">
-        <v>319</v>
+        <v>280</v>
       </c>
       <c r="C84" s="24">
         <v>0</v>
@@ -17555,7 +17537,7 @@
         <v>84</v>
       </c>
       <c r="B85" s="23" t="s">
-        <v>320</v>
+        <v>281</v>
       </c>
       <c r="C85" s="24">
         <v>0</v>
@@ -17638,7 +17620,7 @@
         <v>85</v>
       </c>
       <c r="B86" s="23" t="s">
-        <v>321</v>
+        <v>282</v>
       </c>
       <c r="C86" s="24">
         <v>0</v>
@@ -17721,7 +17703,7 @@
         <v>86</v>
       </c>
       <c r="B87" s="23" t="s">
-        <v>322</v>
+        <v>283</v>
       </c>
       <c r="C87" s="24">
         <v>0</v>
@@ -17804,7 +17786,7 @@
         <v>87</v>
       </c>
       <c r="B88" s="23" t="s">
-        <v>323</v>
+        <v>284</v>
       </c>
       <c r="C88" s="24">
         <v>0</v>
@@ -17887,7 +17869,7 @@
         <v>88</v>
       </c>
       <c r="B89" s="23" t="s">
-        <v>324</v>
+        <v>285</v>
       </c>
       <c r="C89" s="24">
         <v>0</v>
@@ -17970,7 +17952,7 @@
         <v>89</v>
       </c>
       <c r="B90" s="23" t="s">
-        <v>325</v>
+        <v>286</v>
       </c>
       <c r="C90" s="24">
         <v>0</v>
@@ -18053,7 +18035,7 @@
         <v>90</v>
       </c>
       <c r="B91" s="23" t="s">
-        <v>326</v>
+        <v>287</v>
       </c>
       <c r="C91" s="24">
         <v>0</v>
@@ -18136,7 +18118,7 @@
         <v>91</v>
       </c>
       <c r="B92" s="23" t="s">
-        <v>327</v>
+        <v>288</v>
       </c>
       <c r="C92" s="24">
         <v>1</v>
@@ -18219,7 +18201,7 @@
         <v>92</v>
       </c>
       <c r="B93" s="23" t="s">
-        <v>328</v>
+        <v>289</v>
       </c>
       <c r="C93" s="24">
         <v>0</v>
@@ -18302,7 +18284,7 @@
         <v>93</v>
       </c>
       <c r="B94" s="23" t="s">
-        <v>329</v>
+        <v>290</v>
       </c>
       <c r="C94" s="24">
         <v>1</v>
@@ -18385,7 +18367,7 @@
         <v>94</v>
       </c>
       <c r="B95" s="23" t="s">
-        <v>330</v>
+        <v>291</v>
       </c>
       <c r="C95" s="24">
         <v>1</v>
@@ -18468,7 +18450,7 @@
         <v>95</v>
       </c>
       <c r="B96" s="23" t="s">
-        <v>331</v>
+        <v>292</v>
       </c>
       <c r="C96" s="24">
         <v>1</v>
@@ -18551,7 +18533,7 @@
         <v>96</v>
       </c>
       <c r="B97" s="23" t="s">
-        <v>332</v>
+        <v>293</v>
       </c>
       <c r="C97" s="24">
         <v>1</v>
@@ -18634,7 +18616,7 @@
         <v>97</v>
       </c>
       <c r="B98" s="23" t="s">
-        <v>333</v>
+        <v>294</v>
       </c>
       <c r="C98" s="24">
         <v>1</v>
@@ -18717,7 +18699,7 @@
         <v>98</v>
       </c>
       <c r="B99" s="23" t="s">
-        <v>334</v>
+        <v>295</v>
       </c>
       <c r="C99" s="24">
         <v>1</v>
@@ -18800,7 +18782,7 @@
         <v>99</v>
       </c>
       <c r="B100" s="23" t="s">
-        <v>335</v>
+        <v>296</v>
       </c>
       <c r="C100" s="24">
         <v>1</v>
@@ -18883,7 +18865,7 @@
         <v>100</v>
       </c>
       <c r="B101" s="23" t="s">
-        <v>336</v>
+        <v>297</v>
       </c>
       <c r="C101" s="24">
         <v>1</v>
@@ -18966,7 +18948,7 @@
         <v>101</v>
       </c>
       <c r="B102" s="23" t="s">
-        <v>337</v>
+        <v>298</v>
       </c>
       <c r="C102" s="24">
         <v>1</v>
@@ -19049,7 +19031,7 @@
         <v>102</v>
       </c>
       <c r="B103" s="23" t="s">
-        <v>338</v>
+        <v>299</v>
       </c>
       <c r="C103" s="24">
         <v>0</v>
@@ -19132,7 +19114,7 @@
         <v>103</v>
       </c>
       <c r="B104" s="23" t="s">
-        <v>339</v>
+        <v>300</v>
       </c>
       <c r="C104" s="24">
         <v>0</v>
@@ -19215,7 +19197,7 @@
         <v>104</v>
       </c>
       <c r="B105" s="23" t="s">
-        <v>340</v>
+        <v>301</v>
       </c>
       <c r="C105" s="24">
         <v>0</v>
@@ -19298,7 +19280,7 @@
         <v>105</v>
       </c>
       <c r="B106" s="23" t="s">
-        <v>341</v>
+        <v>302</v>
       </c>
       <c r="C106" s="24">
         <v>0</v>
@@ -19381,7 +19363,7 @@
         <v>106</v>
       </c>
       <c r="B107" s="23" t="s">
-        <v>342</v>
+        <v>303</v>
       </c>
       <c r="C107" s="24">
         <v>0</v>
@@ -19464,7 +19446,7 @@
         <v>107</v>
       </c>
       <c r="B108" s="23" t="s">
-        <v>343</v>
+        <v>304</v>
       </c>
       <c r="C108" s="24">
         <v>0</v>
@@ -19547,7 +19529,7 @@
         <v>108</v>
       </c>
       <c r="B109" s="23" t="s">
-        <v>344</v>
+        <v>305</v>
       </c>
       <c r="C109" s="24">
         <v>0</v>
@@ -19630,7 +19612,7 @@
         <v>109</v>
       </c>
       <c r="B110" s="23" t="s">
-        <v>345</v>
+        <v>306</v>
       </c>
       <c r="C110" s="24">
         <v>0</v>
@@ -19713,7 +19695,7 @@
         <v>110</v>
       </c>
       <c r="B111" s="23" t="s">
-        <v>346</v>
+        <v>307</v>
       </c>
       <c r="C111" s="24">
         <v>0</v>
@@ -19796,7 +19778,7 @@
         <v>111</v>
       </c>
       <c r="B112" s="23" t="s">
-        <v>347</v>
+        <v>308</v>
       </c>
       <c r="C112" s="24">
         <v>0</v>
@@ -19879,7 +19861,7 @@
         <v>112</v>
       </c>
       <c r="B113" s="23" t="s">
-        <v>348</v>
+        <v>309</v>
       </c>
       <c r="C113" s="24">
         <v>0</v>
@@ -19962,7 +19944,7 @@
         <v>113</v>
       </c>
       <c r="B114" s="23" t="s">
-        <v>349</v>
+        <v>310</v>
       </c>
       <c r="C114" s="24">
         <v>0</v>
@@ -20045,7 +20027,7 @@
         <v>114</v>
       </c>
       <c r="B115" s="23" t="s">
-        <v>350</v>
+        <v>311</v>
       </c>
       <c r="C115" s="24">
         <v>0</v>
@@ -20128,7 +20110,7 @@
         <v>115</v>
       </c>
       <c r="B116" s="23" t="s">
-        <v>351</v>
+        <v>312</v>
       </c>
       <c r="C116" s="24">
         <v>0</v>
@@ -20211,7 +20193,7 @@
         <v>116</v>
       </c>
       <c r="B117" s="23" t="s">
-        <v>352</v>
+        <v>313</v>
       </c>
       <c r="C117" s="24">
         <v>0</v>
@@ -20294,7 +20276,7 @@
         <v>117</v>
       </c>
       <c r="B118" s="23" t="s">
-        <v>353</v>
+        <v>314</v>
       </c>
       <c r="C118" s="24">
         <v>0</v>
@@ -20377,7 +20359,7 @@
         <v>118</v>
       </c>
       <c r="B119" s="23" t="s">
-        <v>354</v>
+        <v>315</v>
       </c>
       <c r="C119" s="24">
         <v>0</v>
@@ -20460,7 +20442,7 @@
         <v>119</v>
       </c>
       <c r="B120" s="23" t="s">
-        <v>355</v>
+        <v>316</v>
       </c>
       <c r="C120" s="24">
         <v>0</v>
@@ -20543,7 +20525,7 @@
         <v>120</v>
       </c>
       <c r="B121" s="23" t="s">
-        <v>356</v>
+        <v>317</v>
       </c>
       <c r="C121" s="24">
         <v>0</v>
@@ -20626,7 +20608,7 @@
         <v>121</v>
       </c>
       <c r="B122" s="23" t="s">
-        <v>357</v>
+        <v>318</v>
       </c>
       <c r="C122" s="24">
         <v>0</v>
@@ -20709,7 +20691,7 @@
         <v>122</v>
       </c>
       <c r="B123" s="23" t="s">
-        <v>358</v>
+        <v>319</v>
       </c>
       <c r="C123" s="24">
         <v>0</v>
@@ -20792,7 +20774,7 @@
         <v>123</v>
       </c>
       <c r="B124" s="23" t="s">
-        <v>359</v>
+        <v>320</v>
       </c>
       <c r="C124" s="24">
         <v>0</v>
@@ -20875,7 +20857,7 @@
         <v>124</v>
       </c>
       <c r="B125" s="23" t="s">
-        <v>360</v>
+        <v>321</v>
       </c>
       <c r="C125" s="24">
         <v>0</v>
@@ -20958,7 +20940,7 @@
         <v>125</v>
       </c>
       <c r="B126" s="23" t="s">
-        <v>361</v>
+        <v>322</v>
       </c>
       <c r="C126" s="24">
         <v>0</v>
@@ -21041,7 +21023,7 @@
         <v>126</v>
       </c>
       <c r="B127" s="23" t="s">
-        <v>362</v>
+        <v>323</v>
       </c>
       <c r="C127" s="24">
         <v>0</v>
@@ -21124,7 +21106,7 @@
         <v>127</v>
       </c>
       <c r="B128" s="23" t="s">
-        <v>363</v>
+        <v>324</v>
       </c>
       <c r="C128" s="24">
         <v>0</v>
@@ -21207,7 +21189,7 @@
         <v>128</v>
       </c>
       <c r="B129" s="23" t="s">
-        <v>364</v>
+        <v>325</v>
       </c>
       <c r="C129" s="24">
         <v>0</v>
@@ -21290,7 +21272,7 @@
         <v>129</v>
       </c>
       <c r="B130" s="23" t="s">
-        <v>365</v>
+        <v>326</v>
       </c>
       <c r="C130" s="24">
         <v>0</v>
@@ -21373,7 +21355,7 @@
         <v>130</v>
       </c>
       <c r="B131" s="23" t="s">
-        <v>366</v>
+        <v>327</v>
       </c>
       <c r="C131" s="24">
         <v>0</v>
@@ -21456,7 +21438,7 @@
         <v>131</v>
       </c>
       <c r="B132" s="23" t="s">
-        <v>367</v>
+        <v>328</v>
       </c>
       <c r="C132" s="24">
         <v>1</v>
@@ -21539,7 +21521,7 @@
         <v>132</v>
       </c>
       <c r="B133" s="23" t="s">
-        <v>368</v>
+        <v>329</v>
       </c>
       <c r="C133" s="24">
         <v>0</v>
@@ -21622,7 +21604,7 @@
         <v>133</v>
       </c>
       <c r="B134" s="23" t="s">
-        <v>369</v>
+        <v>330</v>
       </c>
       <c r="C134" s="24">
         <v>0</v>
@@ -21705,7 +21687,7 @@
         <v>134</v>
       </c>
       <c r="B135" s="23" t="s">
-        <v>269</v>
+        <v>230</v>
       </c>
       <c r="C135" s="24">
         <v>0</v>
@@ -21788,7 +21770,7 @@
         <v>135</v>
       </c>
       <c r="B136" s="23" t="s">
-        <v>370</v>
+        <v>331</v>
       </c>
       <c r="C136" s="24">
         <v>0</v>
@@ -21871,7 +21853,7 @@
         <v>136</v>
       </c>
       <c r="B137" s="23" t="s">
-        <v>371</v>
+        <v>332</v>
       </c>
       <c r="C137" s="24">
         <v>0</v>
@@ -21954,7 +21936,7 @@
         <v>137</v>
       </c>
       <c r="B138" s="23" t="s">
-        <v>372</v>
+        <v>333</v>
       </c>
       <c r="C138" s="24">
         <v>0</v>
@@ -22037,7 +22019,7 @@
         <v>138</v>
       </c>
       <c r="B139" s="23" t="s">
-        <v>373</v>
+        <v>334</v>
       </c>
       <c r="C139" s="24">
         <v>0</v>
@@ -22120,7 +22102,7 @@
         <v>139</v>
       </c>
       <c r="B140" s="23" t="s">
-        <v>374</v>
+        <v>335</v>
       </c>
       <c r="C140" s="24">
         <v>0</v>
@@ -22203,7 +22185,7 @@
         <v>140</v>
       </c>
       <c r="B141" s="23" t="s">
-        <v>375</v>
+        <v>336</v>
       </c>
       <c r="C141" s="24">
         <v>0</v>
@@ -22286,7 +22268,7 @@
         <v>141</v>
       </c>
       <c r="B142" s="23" t="s">
-        <v>376</v>
+        <v>337</v>
       </c>
       <c r="C142" s="24">
         <v>0</v>
@@ -22369,7 +22351,7 @@
         <v>142</v>
       </c>
       <c r="B143" s="23" t="s">
-        <v>377</v>
+        <v>338</v>
       </c>
       <c r="C143" s="24">
         <v>0</v>
@@ -22452,7 +22434,7 @@
         <v>143</v>
       </c>
       <c r="B144" s="23" t="s">
-        <v>378</v>
+        <v>339</v>
       </c>
       <c r="C144" s="24">
         <v>0</v>
@@ -22535,7 +22517,7 @@
         <v>144</v>
       </c>
       <c r="B145" s="23" t="s">
-        <v>379</v>
+        <v>340</v>
       </c>
       <c r="C145" s="24">
         <v>0</v>
@@ -22618,7 +22600,7 @@
         <v>145</v>
       </c>
       <c r="B146" s="23" t="s">
-        <v>380</v>
+        <v>341</v>
       </c>
       <c r="C146" s="24">
         <v>0</v>
@@ -22701,7 +22683,7 @@
         <v>146</v>
       </c>
       <c r="B147" s="23" t="s">
-        <v>381</v>
+        <v>342</v>
       </c>
       <c r="C147" s="24">
         <v>0</v>
@@ -22784,7 +22766,7 @@
         <v>147</v>
       </c>
       <c r="B148" s="23" t="s">
-        <v>382</v>
+        <v>343</v>
       </c>
       <c r="C148" s="24">
         <v>0</v>
@@ -22867,7 +22849,7 @@
         <v>148</v>
       </c>
       <c r="B149" s="23" t="s">
-        <v>383</v>
+        <v>344</v>
       </c>
       <c r="C149" s="24">
         <v>0</v>
@@ -22950,7 +22932,7 @@
         <v>149</v>
       </c>
       <c r="B150" s="23" t="s">
-        <v>384</v>
+        <v>345</v>
       </c>
       <c r="C150" s="24">
         <v>0</v>
@@ -23033,7 +23015,7 @@
         <v>150</v>
       </c>
       <c r="B151" s="23" t="s">
-        <v>385</v>
+        <v>346</v>
       </c>
       <c r="C151" s="24">
         <v>0</v>
@@ -23116,7 +23098,7 @@
         <v>151</v>
       </c>
       <c r="B152" s="23" t="s">
-        <v>386</v>
+        <v>347</v>
       </c>
       <c r="C152" s="24">
         <v>0</v>
@@ -23199,7 +23181,7 @@
         <v>152</v>
       </c>
       <c r="B153" s="23" t="s">
-        <v>387</v>
+        <v>348</v>
       </c>
       <c r="C153" s="24">
         <v>0</v>
@@ -23282,7 +23264,7 @@
         <v>153</v>
       </c>
       <c r="B154" s="23" t="s">
-        <v>388</v>
+        <v>349</v>
       </c>
       <c r="C154" s="24">
         <v>0</v>
@@ -23365,7 +23347,7 @@
         <v>154</v>
       </c>
       <c r="B155" s="23" t="s">
-        <v>389</v>
+        <v>350</v>
       </c>
       <c r="C155" s="24">
         <v>0</v>
@@ -23448,7 +23430,7 @@
         <v>155</v>
       </c>
       <c r="B156" s="23" t="s">
-        <v>390</v>
+        <v>351</v>
       </c>
       <c r="C156" s="24">
         <v>0</v>
@@ -23531,7 +23513,7 @@
         <v>156</v>
       </c>
       <c r="B157" s="23" t="s">
-        <v>391</v>
+        <v>352</v>
       </c>
       <c r="C157" s="24">
         <v>0</v>
@@ -23614,7 +23596,7 @@
         <v>157</v>
       </c>
       <c r="B158" s="23" t="s">
-        <v>392</v>
+        <v>353</v>
       </c>
       <c r="C158" s="24">
         <v>0</v>
@@ -23697,7 +23679,7 @@
         <v>158</v>
       </c>
       <c r="B159" s="23" t="s">
-        <v>393</v>
+        <v>354</v>
       </c>
       <c r="C159" s="24">
         <v>0</v>
@@ -23780,7 +23762,7 @@
         <v>159</v>
       </c>
       <c r="B160" s="23" t="s">
-        <v>394</v>
+        <v>355</v>
       </c>
       <c r="C160" s="24">
         <v>0</v>
@@ -23863,7 +23845,7 @@
         <v>160</v>
       </c>
       <c r="B161" s="23" t="s">
-        <v>395</v>
+        <v>356</v>
       </c>
       <c r="C161" s="24">
         <v>0</v>
@@ -23946,7 +23928,7 @@
         <v>161</v>
       </c>
       <c r="B162" s="23" t="s">
-        <v>396</v>
+        <v>357</v>
       </c>
       <c r="C162" s="24">
         <v>0</v>
@@ -24029,7 +24011,7 @@
         <v>162</v>
       </c>
       <c r="B163" s="23" t="s">
-        <v>397</v>
+        <v>358</v>
       </c>
       <c r="C163" s="24">
         <v>0</v>
@@ -24112,7 +24094,7 @@
         <v>163</v>
       </c>
       <c r="B164" s="23" t="s">
-        <v>398</v>
+        <v>359</v>
       </c>
       <c r="C164" s="24">
         <v>0</v>
@@ -24195,7 +24177,7 @@
         <v>164</v>
       </c>
       <c r="B165" s="23" t="s">
-        <v>365</v>
+        <v>326</v>
       </c>
       <c r="C165" s="24">
         <v>0</v>
@@ -24278,7 +24260,7 @@
         <v>165</v>
       </c>
       <c r="B166" s="23" t="s">
-        <v>399</v>
+        <v>360</v>
       </c>
       <c r="C166" s="24">
         <v>0</v>
@@ -24361,7 +24343,7 @@
         <v>166</v>
       </c>
       <c r="B167" s="23" t="s">
-        <v>400</v>
+        <v>361</v>
       </c>
       <c r="C167" s="24">
         <v>0</v>
@@ -24444,7 +24426,7 @@
         <v>167</v>
       </c>
       <c r="B168" s="23" t="s">
-        <v>401</v>
+        <v>362</v>
       </c>
       <c r="C168" s="24">
         <v>0</v>
@@ -24527,7 +24509,7 @@
         <v>168</v>
       </c>
       <c r="B169" s="23" t="s">
-        <v>402</v>
+        <v>363</v>
       </c>
       <c r="C169" s="24">
         <v>1</v>
@@ -24610,7 +24592,7 @@
         <v>169</v>
       </c>
       <c r="B170" s="23" t="s">
-        <v>403</v>
+        <v>364</v>
       </c>
       <c r="C170" s="24">
         <v>0</v>
@@ -24693,7 +24675,7 @@
         <v>170</v>
       </c>
       <c r="B171" s="23" t="s">
-        <v>268</v>
+        <v>229</v>
       </c>
       <c r="C171" s="24">
         <v>0</v>
@@ -24776,7 +24758,7 @@
         <v>171</v>
       </c>
       <c r="B172" s="23" t="s">
-        <v>269</v>
+        <v>230</v>
       </c>
       <c r="C172" s="24">
         <v>0</v>
@@ -24885,7 +24867,7 @@
     </row>
     <row r="174" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A174" s="41" t="s">
-        <v>213</v>
+        <v>174</v>
       </c>
       <c r="B174" s="42"/>
       <c r="C174" s="25">
@@ -25022,7 +25004,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="30" t="s">
-        <v>213</v>
+        <v>174</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -25272,14 +25254,14 @@
         <v>2</v>
       </c>
       <c r="F1" s="33" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G1" s="33"/>
       <c r="H1" s="33"/>
       <c r="I1" s="33"/>
       <c r="J1" s="33"/>
       <c r="K1" s="36" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="L1" s="37"/>
       <c r="M1" s="37"/>
@@ -28972,7 +28954,7 @@
     </row>
     <row r="29" spans="1:17" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A29" s="46" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B29" s="47"/>
       <c r="C29" s="47"/>
@@ -28996,7 +28978,7 @@
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="P32" s="32" t="s">
-        <v>404</v>
+        <v>365</v>
       </c>
       <c r="Q32" s="15">
         <f>MIN(Q3:Q27)</f>
@@ -29005,7 +28987,7 @@
     </row>
     <row r="33" spans="16:17" x14ac:dyDescent="0.25">
       <c r="P33" s="32" t="s">
-        <v>405</v>
+        <v>366</v>
       </c>
       <c r="Q33" s="15">
         <f>MAX(Q3:Q27)</f>
@@ -29067,7 +29049,7 @@
         <v>3</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E1" s="19" t="s">
         <v>2</v>
@@ -31890,7 +31872,7 @@
     </row>
     <row r="28" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A28" s="46" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B28" s="47"/>
       <c r="C28" s="47"/>
@@ -31905,7 +31887,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G31" s="32" t="s">
-        <v>404</v>
+        <v>365</v>
       </c>
       <c r="H31" s="15">
         <f>MIN(H2:H26)</f>
@@ -31914,7 +31896,7 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G32" s="32" t="s">
-        <v>405</v>
+        <v>366</v>
       </c>
       <c r="H32" s="15">
         <f>MAX(H2:H26)</f>
@@ -31965,7 +31947,7 @@
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -34787,7 +34769,7 @@
     </row>
     <row r="28" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A28" s="51" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B28" s="51"/>
       <c r="C28" s="51"/>
@@ -34805,7 +34787,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G31" s="32" t="s">
-        <v>404</v>
+        <v>365</v>
       </c>
       <c r="H31" s="15">
         <f>MIN(H2:H26)</f>
@@ -34814,7 +34796,7 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G32" s="32" t="s">
-        <v>405</v>
+        <v>366</v>
       </c>
       <c r="H32" s="15">
         <f>MAX(H2:H26)</f>
@@ -34835,9 +34817,9 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N11" sqref="N11"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O36" sqref="O36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34846,7 +34828,7 @@
     <col min="2" max="2" width="22.85546875" customWidth="1"/>
     <col min="3" max="5" width="22.85546875" hidden="1" customWidth="1"/>
     <col min="6" max="8" width="14.7109375" customWidth="1"/>
-    <col min="9" max="11" width="15.28515625" style="2" customWidth="1"/>
+    <col min="9" max="11" width="13.7109375" style="2" customWidth="1"/>
     <col min="12" max="12" width="34.7109375" style="2" customWidth="1"/>
     <col min="15" max="16" width="23.5703125" customWidth="1"/>
     <col min="17" max="17" width="19.42578125" customWidth="1"/>
@@ -34863,7 +34845,7 @@
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -34878,13 +34860,13 @@
         <v>28</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>167</v>
+        <v>128</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>168</v>
+        <v>129</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>169</v>
+        <v>130</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>23</v>
@@ -34996,26 +34978,26 @@
 Universitas Pendidikan Ganesha menyediakan berbagai jenis beasiswa untuk mendukung mahasiswa berprestasi maupun mahasiswa kurang mampu.</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>160</v>
+        <v>122</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="I2" s="4">
-        <v>0.71851097526223429</v>
+        <v>0.71863784061355684</v>
       </c>
       <c r="J2" s="4">
-        <v>0.57400950636733272</v>
+        <v>0.57391261858257792</v>
       </c>
       <c r="K2" s="4">
-        <v>0.99259456131663648</v>
+        <v>0.99257895071409796</v>
       </c>
       <c r="L2" s="7">
         <f>IFERROR(AVERAGE(I2:K2),0)</f>
-        <v>0.76170501431540105</v>
+        <v>0.76170980330341098</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -35101,26 +35083,26 @@
 Jika Anda memiliki pertanyaan lebih lanjut atau membutuhkan informasi spesifik, silakan tanyakan!</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="I3" s="4">
-        <v>0.63398969710269693</v>
+        <v>0.63388850616985226</v>
       </c>
       <c r="J3" s="4">
-        <v>0.98225009655464013</v>
+        <v>0.98222316514719432</v>
       </c>
       <c r="K3" s="4">
-        <v>0.81323665916515109</v>
+        <v>0.81312324737404018</v>
       </c>
       <c r="L3" s="7">
         <f t="shared" ref="L3:L26" si="0">IFERROR(AVERAGE(I3:K3),0)</f>
-        <v>0.80982548427416268</v>
+        <v>0.80974497289702896</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -35208,26 +35190,26 @@
 Anda dapat melihat informasi daya tampung mahasiswa baru Universitas Pendidikan Ganesha tahun akademik 2024/2025 dengan mengunjungi tautan berikut: [Daya Tampung Mahasiswa Baru 2024/2025](https://undiksha.ac.id/pmb/tahun2024/daya-tampung/).</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="I4" s="4">
-        <v>0.85263439567443</v>
+        <v>0.85265819514290009</v>
       </c>
       <c r="J4" s="4">
-        <v>0.67934954361236399</v>
+        <v>0.67692835187430178</v>
       </c>
       <c r="K4" s="4">
-        <v>0.97867629004299117</v>
+        <v>0.97594704494944196</v>
       </c>
       <c r="L4" s="7">
         <f t="shared" si="0"/>
-        <v>0.83688674310992839</v>
+        <v>0.83517786398888127</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -35357,26 +35339,26 @@
 Daya tampung mahasiswa untuk Program Studi Ilmu Komputer (S1) di Universitas Pendidikan Ganesha adalah 110.</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>162</v>
+        <v>124</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>161</v>
+        <v>123</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="I5" s="4">
-        <v>0.83679804265726865</v>
+        <v>0.83908751611818944</v>
       </c>
       <c r="J5" s="4">
-        <v>0.78558497392701299</v>
+        <v>0.7842503890523923</v>
       </c>
       <c r="K5" s="4">
-        <v>0.97081778216779702</v>
+        <v>0.97012458390471368</v>
       </c>
       <c r="L5" s="7">
         <f t="shared" si="0"/>
-        <v>0.86440026625069288</v>
+        <v>0.86448749635843181</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -35473,26 +35455,26 @@
 Jika ada pertanyaan lebih lanjut, silakan tanyakan!</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>163</v>
+        <v>125</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>33</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="I6" s="4">
-        <v>0.80743659739000839</v>
+        <v>0.80759181699616889</v>
       </c>
       <c r="J6" s="4">
-        <v>0.99999872724177241</v>
+        <v>1</v>
       </c>
       <c r="K6" s="4">
-        <v>0.84669630445282174</v>
+        <v>0.84690250182064586</v>
       </c>
       <c r="L6" s="7">
         <f t="shared" si="0"/>
-        <v>0.88471054302820085</v>
+        <v>0.88483143960560495</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -35584,26 +35566,26 @@
 Estimasi biaya kuliah adalah perkiraan biaya yang harus ditanggung oleh calon mahasiswa per semester untuk mengikuti perkuliahan di Universitas Pendidikan Ganesha (Undiksha). Biaya ini mencakup berbagai komponen, seperti biaya pendidikan, biaya administrasi, dan biaya lainnya yang mungkin diperlukan selama proses perkuliahan. Estimasi ini penting untuk membantu calon mahasiswa merencanakan keuangan mereka selama menempuh pendidikan di Undiksha.</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="I7" s="4">
-        <v>0.95746545948414052</v>
+        <v>0.95679993412534114</v>
       </c>
       <c r="J7" s="4">
-        <v>0.63899285125630156</v>
+        <v>0.63820647679934361</v>
       </c>
       <c r="K7" s="4">
-        <v>0.66116007961474155</v>
+        <v>0.66005565679951894</v>
       </c>
       <c r="L7" s="7">
         <f t="shared" si="0"/>
-        <v>0.75253946345172784</v>
+        <v>0.7516873559080679</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -35716,26 +35698,26 @@
 Fasilitas-fasilitas ini dirancang untuk mendukung kegiatan akademik dan non-akademik mahasiswa di Universitas Pendidikan Ganesha.</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>164</v>
+        <v>126</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I8" s="4">
-        <v>0.80288984253684315</v>
+        <v>0.80180036669069865</v>
       </c>
       <c r="J8" s="4">
-        <v>0.98650429819918339</v>
+        <v>0.98657221451013921</v>
       </c>
       <c r="K8" s="4">
-        <v>0.87101185171055751</v>
+        <v>0.87161556948077357</v>
       </c>
       <c r="L8" s="7">
         <f t="shared" si="0"/>
-        <v>0.88680199748219468</v>
+        <v>0.88666271689387044</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -35839,26 +35821,26 @@
 Anda dapat mendapatkan informasi mengenai fasilitas layanan konseling di Universitas Pendidikan Ganesha dengan menghubungi unit konseling. Anda bisa menghubungi nomor informasi berikut: (+6281246318813). Di sana, Anda akan mendapatkan penjelasan lebih lanjut mengenai layanan yang tersedia.</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>165</v>
+        <v>127</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="I9" s="4">
-        <v>0.70499335675751873</v>
+        <v>0.70507111539311473</v>
       </c>
       <c r="J9" s="4">
-        <v>0.74097428963356093</v>
+        <v>0.74098453852588619</v>
       </c>
       <c r="K9" s="4">
-        <v>0.9746483471305819</v>
+        <v>0.97474208323902112</v>
       </c>
       <c r="L9" s="7">
         <f t="shared" si="0"/>
-        <v>0.80687199784055386</v>
+        <v>0.80693257905267401</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -35975,23 +35957,23 @@
         <v>37</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="I10" s="4">
-        <v>0.99999884088833302</v>
+        <v>0.99999868063006858</v>
       </c>
       <c r="J10" s="4">
-        <v>0.97207992813888155</v>
+        <v>0.97203066351213552</v>
       </c>
       <c r="K10" s="4">
-        <v>0.84786157977474808</v>
+        <v>0.84775617049270635</v>
       </c>
       <c r="L10" s="7">
         <f t="shared" si="0"/>
-        <v>0.93998011626732092</v>
+        <v>0.93992850487830337</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -36129,26 +36111,26 @@
 Untuk informasi lebih lanjut, Anda dapat melihat video profil Fakultas Bahasa dan Seni [di sini](https://youtu.be/DeLKu41DVn0).</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="I11" s="4">
-        <v>0.91685376598194201</v>
+        <v>0.91681112377427376</v>
       </c>
       <c r="J11" s="4">
-        <v>0.91146521955325421</v>
+        <v>0.91105317439450295</v>
       </c>
       <c r="K11" s="4">
-        <v>0.97743584655551841</v>
+        <v>0.97747549234113962</v>
       </c>
       <c r="L11" s="7">
         <f t="shared" si="0"/>
-        <v>0.93525161069690499</v>
+        <v>0.93511326350330537</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -36242,26 +36224,26 @@
 Ya, Fakultas Hukum dan Ilmu Sosial (FHIS) Universitas Pendidikan Ganesha memiliki video profil. Anda dapat menontonnya melalui tautan berikut: [Video Profil FHIS Undiksha](https://youtu.be/xrruGWs5HNk). Video ini memberikan informasi mengenai fakultas, program studi, dan berbagai kegiatan yang ada di FHIS.</v>
       </c>
       <c r="F12" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="H12" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="G12" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>123</v>
-      </c>
       <c r="I12" s="4">
-        <v>0.99999916495249463</v>
+        <v>0.91951203871346665</v>
       </c>
       <c r="J12" s="4">
-        <v>0.81456933031344625</v>
+        <v>0.74376824364288874</v>
       </c>
       <c r="K12" s="4">
-        <v>0.86182004375428245</v>
+        <v>0.99999908286431016</v>
       </c>
       <c r="L12" s="7">
         <f t="shared" si="0"/>
-        <v>0.89212951300674115</v>
+        <v>0.88775978840688852</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -36360,26 +36342,26 @@
 Dengan demikian, pengembangan kurikulum di Undiksha bertujuan untuk menghasilkan lulusan yang berkualitas dan siap bersaing di dunia kerja.</v>
       </c>
       <c r="F13" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="G13" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="G13" s="5" t="s">
-        <v>124</v>
-      </c>
       <c r="H13" s="5" t="s">
-        <v>40</v>
+        <v>119</v>
       </c>
       <c r="I13" s="4">
-        <v>0.70889882841642027</v>
+        <v>0.88384442467033564</v>
       </c>
       <c r="J13" s="4">
-        <v>0.81679710638981995</v>
+        <v>0.88646629454938008</v>
       </c>
       <c r="K13" s="4">
-        <v>0.999998753773371</v>
+        <v>0.92157838993894803</v>
       </c>
       <c r="L13" s="7">
         <f t="shared" si="0"/>
-        <v>0.84189822952653703</v>
+        <v>0.89729636971955451</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -36482,26 +36464,26 @@
 Informasi lebih lanjut mengenai prosedur pembayaran Uang Kuliah Tunggal (UKT) dengan layanan BRI Virtual Account (BRIVA) dapat ditemukan di situs resmi Universitas Pendidikan Ganesha melalui tautan berikut: [Prosedur Pembayaran UKT Mahasiswa Baru Undiksha](https://undiksha.ac.id/prosedur-pembayaran-ukt-mahasiswa-baru-undiksha-dengan-layanan-bri-virtual-account-briva/).</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>126</v>
+        <v>368</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>125</v>
+        <v>369</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>127</v>
+        <v>370</v>
       </c>
       <c r="I14" s="4">
-        <v>0.73455558948689359</v>
+        <v>0.66469443341301115</v>
       </c>
       <c r="J14" s="4">
-        <v>0.79012014400078334</v>
+        <v>0.97497875645418697</v>
       </c>
       <c r="K14" s="4">
-        <v>0.68504634427974564</v>
+        <v>0.65517740391141399</v>
       </c>
       <c r="L14" s="7">
         <f t="shared" si="0"/>
-        <v>0.73657402592247434</v>
+        <v>0.76495019792620411</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -36638,26 +36620,26 @@
 9. Membayar biaya UTBK (kecuali peserta KIP Kuliah).</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>128</v>
+        <v>371</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>129</v>
+        <v>372</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>41</v>
+        <v>373</v>
       </c>
       <c r="I15" s="4">
-        <v>0.91940527532188354</v>
+        <v>0.86969111566595714</v>
       </c>
       <c r="J15" s="4">
-        <v>0.74374201013075392</v>
+        <v>0.98105094045105479</v>
       </c>
       <c r="K15" s="4">
-        <v>0.99999933354481896</v>
+        <v>0.94611697512705939</v>
       </c>
       <c r="L15" s="7">
         <f t="shared" si="0"/>
-        <v>0.88771553966581873</v>
+        <v>0.93228634374802377</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -36750,26 +36732,26 @@
 Jadwal pendaftaran seleksi mahasiswa baru jalur mandiri (SMBJM) Universitas Pendidikan Ganesha untuk tahun 2025 akan diinformasikan segera. Mohon untuk selalu memantau informasi resmi dari Undiksha untuk mendapatkan update terkini.</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>130</v>
+        <v>374</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>131</v>
+        <v>43</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>132</v>
+        <v>375</v>
       </c>
       <c r="I16" s="4">
-        <v>0.80210401758350769</v>
+        <v>0.84366039819849492</v>
       </c>
       <c r="J16" s="4">
-        <v>0.86789705690993957</v>
+        <v>0.9999990442932194</v>
       </c>
       <c r="K16" s="4">
-        <v>0.75194966905732308</v>
+        <v>0.75894382780893255</v>
       </c>
       <c r="L16" s="7">
         <f t="shared" si="0"/>
-        <v>0.80731691451692333</v>
+        <v>0.86753442343354903</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -36886,26 +36868,26 @@
 Untuk informasi lebih lanjut mengenai pendaftaran ulang bagi peserta yang lulus SNBP, dapat dilihat pada laman masing-masing PTN yang dituju.</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>133</v>
+        <v>44</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>134</v>
+        <v>376</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>135</v>
+        <v>377</v>
       </c>
       <c r="I17" s="4">
-        <v>0.81459532841910676</v>
+        <v>0.99999910781491586</v>
       </c>
       <c r="J17" s="4">
-        <v>0.96359529368819141</v>
+        <v>0.88739126970701288</v>
       </c>
       <c r="K17" s="4">
-        <v>0.98508925451134755</v>
+        <v>0.88312316365971522</v>
       </c>
       <c r="L17" s="7">
         <f t="shared" si="0"/>
-        <v>0.92109329220621516</v>
+        <v>0.92350451372721454</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -37020,26 +37002,26 @@
 5. Memenuhi persyaratan yang ditentukan oleh masing-masing PTN Akademik dan PTN Vokasi.</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>166</v>
+        <v>378</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>42</v>
+        <v>379</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>136</v>
+        <v>45</v>
       </c>
       <c r="I18" s="4">
-        <v>0.68778765013690857</v>
+        <v>0.93564647905741005</v>
       </c>
       <c r="J18" s="4">
+        <v>0.90209484743098645</v>
+      </c>
+      <c r="K18" s="4">
         <v>1</v>
-      </c>
-      <c r="K18" s="4">
-        <v>0.83935975738224944</v>
       </c>
       <c r="L18" s="7">
         <f t="shared" si="0"/>
-        <v>0.84238246917305259</v>
+        <v>0.9459137754961322</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -37151,26 +37133,26 @@
 4. Masa Unduh Sertifikat UTBK: 03 Juni – 31 Juli 2025.</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>137</v>
+        <v>46</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>138</v>
+        <v>380</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>139</v>
+        <v>381</v>
       </c>
       <c r="I19" s="4">
-        <v>0.95119631223481382</v>
+        <v>0.99999908678709559</v>
       </c>
       <c r="J19" s="4">
-        <v>0.95969803208392712</v>
+        <v>0.84773545836858799</v>
       </c>
       <c r="K19" s="4">
-        <v>0.81487363646416644</v>
+        <v>0.89302359627191064</v>
       </c>
       <c r="L19" s="7">
         <f t="shared" si="0"/>
-        <v>0.90858932692763583</v>
+        <v>0.91358604714253155</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -37265,26 +37247,26 @@
 Biaya untuk mengikuti Seleksi Nasional Berbasis Tes (SNBT) sebesar Rp200.000,00 (dua ratus ribu rupiah). Pembayaran dapat dilakukan melalui mitra bank seperti Mandiri, BNI, BTN, BRI, dan BSI.</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>43</v>
+        <v>382</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>140</v>
+        <v>383</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>141</v>
+        <v>384</v>
       </c>
       <c r="I20" s="4">
-        <v>0.99999879815464598</v>
+        <v>0.93232993625611338</v>
       </c>
       <c r="J20" s="4">
-        <v>0.96894380154297011</v>
+        <v>0.97787619619617772</v>
       </c>
       <c r="K20" s="4">
-        <v>0.98284456119727803</v>
+        <v>0.90103685434839742</v>
       </c>
       <c r="L20" s="7">
         <f t="shared" si="0"/>
-        <v>0.98392905363163141</v>
+        <v>0.93708099560022939</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -37393,26 +37375,26 @@
 Fungsi utama Unit Kegiatan Mahasiswa (UKM) di Universitas Pendidikan Ganesha adalah sebagai wadah aktivitas kemahasiswaan untuk mengembangkan minat, bakat, dan keahlian tertentu bagi para anggotanya. Selain itu, UKM juga berperan sebagai partner organisasi kemahasiswaan intra kampus lainnya, seperti Badan Eksekutif Mahasiswa. UKM bersifat otonom, yang berarti UKM tidak merupakan bagian dari Badan Eksekutif Mahasiswa.</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>142</v>
+        <v>385</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>143</v>
+        <v>386</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>144</v>
+        <v>387</v>
       </c>
       <c r="I21" s="4">
-        <v>0.95235811537844794</v>
+        <v>0.84748010942805629</v>
       </c>
       <c r="J21" s="4">
-        <v>0.81900866839372355</v>
+        <v>0.99005616585936729</v>
       </c>
       <c r="K21" s="4">
-        <v>0.94635868336290629</v>
+        <v>0.89999648737023286</v>
       </c>
       <c r="L21" s="7">
         <f t="shared" si="0"/>
-        <v>0.90590848904502597</v>
+        <v>0.91251092088588548</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -37526,26 +37508,26 @@
 Untuk mendapatkan informasi lebih lanjut tentang Unit Kegiatan Mahasiswa (UKM) di Universitas Pendidikan Ganesha, Anda dapat mengunjungi situs resmi UKM Undiksha di link berikut: [UKM Undiksha](https://undiksha.ac.id/kemahasiswaan/ukm/). Di sana, Anda akan menemukan informasi mengenai berbagai UKM yang ada, termasuk kegiatan, tujuan, dan cara bergabung.</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>145</v>
+        <v>388</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>146</v>
+        <v>389</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>147</v>
+        <v>390</v>
       </c>
       <c r="I22" s="4">
-        <v>0.95899259792947289</v>
+        <v>0.81315886299249795</v>
       </c>
       <c r="J22" s="4">
-        <v>0.88896052744723941</v>
+        <v>0.98984704469301499</v>
       </c>
       <c r="K22" s="4">
-        <v>0.869152533344145</v>
+        <v>0.95670509813718463</v>
       </c>
       <c r="L22" s="7">
         <f t="shared" si="0"/>
-        <v>0.9057018862402858</v>
+        <v>0.91990366860756589</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -37634,26 +37616,26 @@
 Motto Universitas Pendidikan Ganesha (Undiksha) adalah “dharmaning sajjana umerdhyaken widyaguna” yang berarti kewajiban orang bijaksana adalah mengembangkan ilmu pengetahuan dan pekerti.</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>148</v>
+        <v>391</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>149</v>
+        <v>392</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>150</v>
+        <v>393</v>
       </c>
       <c r="I23" s="4">
-        <v>0.97037868093137847</v>
+        <v>0.7464879782802416</v>
       </c>
       <c r="J23" s="4">
-        <v>0.83853449535206503</v>
+        <v>0.72397787927997548</v>
       </c>
       <c r="K23" s="4">
-        <v>0.83353814309796359</v>
+        <v>0.70152191784474438</v>
       </c>
       <c r="L23" s="7">
         <f t="shared" si="0"/>
-        <v>0.88081710646046896</v>
+        <v>0.72399592513498712</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -37737,26 +37719,26 @@
 Dengan demikian, Undiksha menjadi satu-satunya perguruan tinggi negeri di Bali Utara yang memiliki akreditasi A dan diakui secara internasional.</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>152</v>
+        <v>51</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>151</v>
+        <v>394</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>153</v>
+        <v>395</v>
       </c>
       <c r="I24" s="4">
-        <v>0.98541505648305294</v>
+        <v>0.99999999999999978</v>
       </c>
       <c r="J24" s="4">
-        <v>0.7883865281671999</v>
+        <v>0.61429050700020571</v>
       </c>
       <c r="K24" s="4">
-        <v>0.93816578372357884</v>
+        <v>0.65251031352461397</v>
       </c>
       <c r="L24" s="7">
         <f t="shared" si="0"/>
-        <v>0.90398912279127719</v>
+        <v>0.75560027350827319</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -37850,26 +37832,26 @@
 Visi Universitas Pendidikan Ganesha (Undiksha) adalah menjadi Universitas Unggul Berlandaskan Falsafah Tri Hita Karana di Asia Pada Tahun 2045. Visi ini mencerminkan komitmen Undiksha untuk mencapai keunggulan dengan mengedepankan nilai-nilai yang terkandung dalam falsafah Tri Hita Karana.</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>154</v>
+        <v>396</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>155</v>
+        <v>397</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>156</v>
+        <v>52</v>
       </c>
       <c r="I25" s="4">
-        <v>0.95909082456105632</v>
+        <v>0.72720318866597433</v>
       </c>
       <c r="J25" s="4">
-        <v>0.84223654566915118</v>
+        <v>0.85721793308367489</v>
       </c>
       <c r="K25" s="4">
-        <v>0.93701079547470167</v>
+        <v>0.99999895418005169</v>
       </c>
       <c r="L25" s="7">
         <f t="shared" si="0"/>
-        <v>0.91277938856830299</v>
+        <v>0.8614733586432336</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -37963,26 +37945,26 @@
 Rektor Universitas Pendidikan Ganesha saat ini adalah Prof. Dr. I Wayan Lasmawan, M.Pd.</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>158</v>
+        <v>398</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>159</v>
+        <v>399</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>157</v>
+        <v>400</v>
       </c>
       <c r="I26" s="4">
-        <v>0.88403011190425518</v>
+        <v>0.67755881799199746</v>
       </c>
       <c r="J26" s="4">
-        <v>0.88652011910706408</v>
+        <v>0.70296417127798638</v>
       </c>
       <c r="K26" s="4">
-        <v>0.92166614884135301</v>
+        <v>0.93692927602033016</v>
       </c>
       <c r="L26" s="7">
         <f t="shared" si="0"/>
-        <v>0.89740545995089072</v>
+        <v>0.77248408843010463</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -38001,7 +37983,7 @@
     </row>
     <row r="28" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A28" s="46" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B28" s="47"/>
       <c r="C28" s="47"/>
@@ -38015,25 +37997,25 @@
       <c r="K28" s="48"/>
       <c r="L28" s="10">
         <f>IFERROR(AVERAGE(L2:L26),0)</f>
-        <v>0.86828812217401496</v>
+        <v>0.8596862674719985</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K31" s="32" t="s">
-        <v>404</v>
+        <v>365</v>
       </c>
       <c r="L31" s="15">
         <f>MIN(L2:L26)</f>
-        <v>0.73657402592247434</v>
+        <v>0.72399592513498712</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K32" s="32" t="s">
-        <v>405</v>
+        <v>366</v>
       </c>
       <c r="L32" s="15">
         <f>MAX(L2:L26)</f>
-        <v>0.98392905363163141</v>
+        <v>0.9459137754961322</v>
       </c>
     </row>
   </sheetData>
@@ -38049,9 +38031,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3728C640-F655-4ACE-93F4-7C1178A6920C}">
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G13" sqref="G13"/>
+      <selection pane="bottomLeft" activeCell="W15" sqref="W15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -38064,33 +38046,33 @@
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="52" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B1" s="54" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C1" s="55"/>
       <c r="D1" s="54" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="E1" s="55"/>
       <c r="F1" s="34" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="53"/>
       <c r="B2" s="14" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="F2" s="35"/>
     </row>
@@ -38112,11 +38094,11 @@
       </c>
       <c r="E3" s="13" cm="1">
         <f t="array" ref="E3:E27">IFERROR(RR!$L2:$L26,0)</f>
-        <v>0.76170501431540105</v>
+        <v>0.76170980330341098</v>
       </c>
       <c r="F3" s="13">
         <f>IFERROR(AVERAGE(B3:E3),0)</f>
-        <v>0.74399768215027884</v>
+        <v>0.74399887939728138</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -38133,11 +38115,11 @@
         <v>0.8571428571428571</v>
       </c>
       <c r="E4" s="13">
-        <v>0.80982548427416268</v>
+        <v>0.80974497289702896</v>
       </c>
       <c r="F4" s="13">
         <f t="shared" ref="F4:F27" si="0">IFERROR(AVERAGE(B4:E4),0)</f>
-        <v>0.79174208535425494</v>
+        <v>0.79172195750997154</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -38154,11 +38136,11 @@
         <v>1</v>
       </c>
       <c r="E5" s="13">
-        <v>0.83688674310992839</v>
+        <v>0.83517786398888127</v>
       </c>
       <c r="F5" s="13">
         <f t="shared" si="0"/>
-        <v>0.95922168577748212</v>
+        <v>0.95879446599722029</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -38175,11 +38157,11 @@
         <v>1</v>
       </c>
       <c r="E6" s="13">
-        <v>0.86440026625069288</v>
+        <v>0.86448749635843181</v>
       </c>
       <c r="F6" s="13">
         <f t="shared" si="0"/>
-        <v>0.84110006656267322</v>
+        <v>0.84112187408960792</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -38196,11 +38178,11 @@
         <v>1</v>
       </c>
       <c r="E7" s="13">
-        <v>0.88471054302820085</v>
+        <v>0.88483143960560495</v>
       </c>
       <c r="F7" s="13">
         <f t="shared" si="0"/>
-        <v>0.97117763575705018</v>
+        <v>0.97120785990140124</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -38217,11 +38199,11 @@
         <v>1</v>
       </c>
       <c r="E8" s="13">
-        <v>0.75253946345172784</v>
+        <v>0.7516873559080679</v>
       </c>
       <c r="F8" s="13">
         <f t="shared" si="0"/>
-        <v>0.93813486586293193</v>
+        <v>0.93792183897701698</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -38238,11 +38220,11 @@
         <v>0.8571428571428571</v>
       </c>
       <c r="E9" s="13">
-        <v>0.88680199748219468</v>
+        <v>0.88666271689387044</v>
       </c>
       <c r="F9" s="13">
         <f t="shared" si="0"/>
-        <v>0.73598621365626293</v>
+        <v>0.73595139350918182</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -38259,11 +38241,11 @@
         <v>1</v>
       </c>
       <c r="E10" s="13">
-        <v>0.80687199784055386</v>
+        <v>0.80693257905267401</v>
       </c>
       <c r="F10" s="13">
         <f t="shared" si="0"/>
-        <v>0.95171799946013846</v>
+        <v>0.9517331447631685</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -38280,11 +38262,11 @@
         <v>1</v>
       </c>
       <c r="E11" s="13">
-        <v>0.93998011626732092</v>
+        <v>0.93992850487830337</v>
       </c>
       <c r="F11" s="13">
         <f t="shared" si="0"/>
-        <v>0.98499502906683023</v>
+        <v>0.98498212621957582</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -38301,11 +38283,11 @@
         <v>0.88461538461538458</v>
       </c>
       <c r="E12" s="13">
-        <v>0.93525161069690499</v>
+        <v>0.93511326350330537</v>
       </c>
       <c r="F12" s="13">
         <f t="shared" si="0"/>
-        <v>0.95496674882807242</v>
+        <v>0.95493216202967246</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -38322,11 +38304,11 @@
         <v>1</v>
       </c>
       <c r="E13" s="13">
-        <v>0.89212951300674115</v>
+        <v>0.88775978840688852</v>
       </c>
       <c r="F13" s="13">
         <f t="shared" si="0"/>
-        <v>0.97303237825168531</v>
+        <v>0.97193994710172216</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -38343,11 +38325,11 @@
         <v>0.6</v>
       </c>
       <c r="E14" s="13">
-        <v>0.84189822952653703</v>
+        <v>0.89729636971955451</v>
       </c>
       <c r="F14" s="13">
         <f t="shared" si="0"/>
-        <v>0.61047455738163425</v>
+        <v>0.62432409242988862</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -38364,11 +38346,11 @@
         <v>1</v>
       </c>
       <c r="E15" s="13">
-        <v>0.73657402592247434</v>
+        <v>0.76495019792620411</v>
       </c>
       <c r="F15" s="13">
         <f t="shared" si="0"/>
-        <v>0.89247683981395187</v>
+        <v>0.89957088281488429</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -38385,11 +38367,11 @@
         <v>0.8</v>
       </c>
       <c r="E16" s="13">
-        <v>0.88771553966581873</v>
+        <v>0.93228634374802377</v>
       </c>
       <c r="F16" s="13">
         <f t="shared" si="0"/>
-        <v>0.88026221824978801</v>
+        <v>0.89140491927033927</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -38406,11 +38388,11 @@
         <v>1</v>
       </c>
       <c r="E17" s="13">
-        <v>0.80731691451692333</v>
+        <v>0.86753442343354903</v>
       </c>
       <c r="F17" s="13">
         <f t="shared" si="0"/>
-        <v>0.82682922862923081</v>
+        <v>0.84188360585838729</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -38427,11 +38409,11 @@
         <v>1</v>
       </c>
       <c r="E18" s="13">
-        <v>0.92109329220621516</v>
+        <v>0.92350451372721454</v>
       </c>
       <c r="F18" s="13">
         <f t="shared" si="0"/>
-        <v>0.66777332305155379</v>
+        <v>0.66837612843180361</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -38448,11 +38430,11 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="E19" s="13">
-        <v>0.84238246917305259</v>
+        <v>0.9459137754961322</v>
       </c>
       <c r="F19" s="13">
         <f t="shared" si="0"/>
-        <v>0.75226228395992978</v>
+        <v>0.77814511054069968</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -38469,11 +38451,11 @@
         <v>0.8</v>
       </c>
       <c r="E20" s="13">
-        <v>0.90858932692763583</v>
+        <v>0.91358604714253155</v>
       </c>
       <c r="F20" s="13">
         <f t="shared" si="0"/>
-        <v>0.80353622062079777</v>
+        <v>0.80478540067452176</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -38490,11 +38472,11 @@
         <v>1</v>
       </c>
       <c r="E21" s="13">
-        <v>0.98392905363163141</v>
+        <v>0.93708099560022939</v>
       </c>
       <c r="F21" s="13">
         <f t="shared" si="0"/>
-        <v>0.99598226340790785</v>
+        <v>0.98427024890005732</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -38511,11 +38493,11 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="E22" s="13">
-        <v>0.90590848904502597</v>
+        <v>0.91251092088588548</v>
       </c>
       <c r="F22" s="13">
         <f t="shared" si="0"/>
-        <v>0.89314378892792312</v>
+        <v>0.894794396888138</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -38532,11 +38514,11 @@
         <v>1</v>
       </c>
       <c r="E23" s="13">
-        <v>0.9057018862402858</v>
+        <v>0.91990366860756589</v>
       </c>
       <c r="F23" s="13">
         <f t="shared" si="0"/>
-        <v>0.97642547156007142</v>
+        <v>0.97997591715189147</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -38553,11 +38535,11 @@
         <v>1</v>
       </c>
       <c r="E24" s="13">
-        <v>0.88081710646046896</v>
+        <v>0.72399592513498712</v>
       </c>
       <c r="F24" s="13">
         <f t="shared" si="0"/>
-        <v>0.92853760994845047</v>
+        <v>0.88933231461708007</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -38574,11 +38556,11 @@
         <v>0.75</v>
       </c>
       <c r="E25" s="13">
-        <v>0.90398912279127719</v>
+        <v>0.75560027350827319</v>
       </c>
       <c r="F25" s="13">
         <f t="shared" si="0"/>
-        <v>0.83016394736448595</v>
+        <v>0.79306673504373493</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -38595,11 +38577,11 @@
         <v>1</v>
       </c>
       <c r="E26" s="13">
-        <v>0.91277938856830299</v>
+        <v>0.8614733586432336</v>
       </c>
       <c r="F26" s="13">
         <f t="shared" si="0"/>
-        <v>0.81152818047540898</v>
+        <v>0.79870167299414163</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -38616,11 +38598,11 @@
         <v>1</v>
       </c>
       <c r="E27" s="13">
-        <v>0.89740545995089072</v>
+        <v>0.77248408843010463</v>
       </c>
       <c r="F27" s="13">
         <f t="shared" si="0"/>
-        <v>0.97435136498772268</v>
+        <v>0.94312102210752613</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -38633,7 +38615,7 @@
     </row>
     <row r="29" spans="1:6" s="17" customFormat="1" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A29" s="18" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B29" s="16">
         <f>IFERROR(AVERAGE(_xlfn.ANCHORARRAY($B$3)),0)</f>
@@ -38649,11 +38631,11 @@
       </c>
       <c r="E29" s="16">
         <f>IFERROR(AVERAGE(_xlfn.ANCHORARRAY($E$3)),0)</f>
-        <v>0.86828812217401496</v>
+        <v>0.8596862674719985</v>
       </c>
       <c r="F29" s="16">
         <f>IFERROR(AVERAGE(B29:E29),0)</f>
-        <v>0.86759278756426084</v>
+        <v>0.86544232388875675</v>
       </c>
     </row>
   </sheetData>

</xml_diff>